<commit_message>
【MS-OXCTABL]: Update capture code for latest RS
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCTABL/MS-OXCTABL_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCTABL/MS-OXCTABL_RequirementSpecification.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6122" uniqueCount="1957">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6128" uniqueCount="1957">
   <si>
     <t>Req ID</t>
   </si>
@@ -6425,21 +6425,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -6463,6 +6448,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7405,127 +7405,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -7538,12 +7538,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -7556,12 +7556,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -7574,12 +7574,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -7592,60 +7592,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="45"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -27366,7 +27366,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="795" spans="1:9" ht="45">
+    <row r="795" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A795" s="22" t="s">
         <v>1921</v>
       </c>
@@ -27385,7 +27385,9 @@
       <c r="F795" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G795" s="33"/>
+      <c r="G795" s="29" t="s">
+        <v>15</v>
+      </c>
       <c r="H795" s="29" t="s">
         <v>20</v>
       </c>
@@ -27393,7 +27395,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="796" spans="1:9" ht="45">
+    <row r="796" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A796" s="22" t="s">
         <v>1922</v>
       </c>
@@ -27412,15 +27414,15 @@
       <c r="F796" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G796" s="33"/>
+      <c r="G796" s="29" t="s">
+        <v>15</v>
+      </c>
       <c r="H796" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I796" s="31" t="s">
-        <v>1593</v>
-      </c>
-    </row>
-    <row r="797" spans="1:9" ht="45">
+        <v>18</v>
+      </c>
+      <c r="I796" s="31"/>
+    </row>
+    <row r="797" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A797" s="22" t="s">
         <v>1923</v>
       </c>
@@ -27439,7 +27441,9 @@
       <c r="F797" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G797" s="33"/>
+      <c r="G797" s="29" t="s">
+        <v>15</v>
+      </c>
       <c r="H797" s="29" t="s">
         <v>20</v>
       </c>
@@ -27447,7 +27451,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="798" spans="1:9" ht="45">
+    <row r="798" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A798" s="22" t="s">
         <v>1924</v>
       </c>
@@ -27466,7 +27470,9 @@
       <c r="F798" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G798" s="33"/>
+      <c r="G798" s="29" t="s">
+        <v>15</v>
+      </c>
       <c r="H798" s="29" t="s">
         <v>20</v>
       </c>
@@ -27474,7 +27480,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="799" spans="1:9" ht="45">
+    <row r="799" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A799" s="22" t="s">
         <v>1925</v>
       </c>
@@ -27493,7 +27499,9 @@
       <c r="F799" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G799" s="33"/>
+      <c r="G799" s="29" t="s">
+        <v>15</v>
+      </c>
       <c r="H799" s="29" t="s">
         <v>20</v>
       </c>
@@ -27501,7 +27509,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="800" spans="1:9" ht="45">
+    <row r="800" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A800" s="22" t="s">
         <v>1926</v>
       </c>
@@ -27520,7 +27528,9 @@
       <c r="F800" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G800" s="33"/>
+      <c r="G800" s="29" t="s">
+        <v>15</v>
+      </c>
       <c r="H800" s="29" t="s">
         <v>20</v>
       </c>
@@ -27528,7 +27538,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="801" spans="1:9" ht="45">
+    <row r="801" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A801" s="22" t="s">
         <v>1927</v>
       </c>
@@ -27547,7 +27557,9 @@
       <c r="F801" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G801" s="33"/>
+      <c r="G801" s="29" t="s">
+        <v>15</v>
+      </c>
       <c r="H801" s="29" t="s">
         <v>20</v>
       </c>
@@ -29033,6 +29045,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -29040,11 +29057,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:I855">

</xml_diff>

<commit_message>
[MS-OXCTABL]: Update for model error
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCTABL/MS-OXCTABL_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCTABL/MS-OXCTABL_RequirementSpecification.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6128" uniqueCount="1957">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6127" uniqueCount="1958">
   <si>
     <t>Req ID</t>
   </si>
@@ -5247,10 +5247,6 @@
     <t>[In Appendix A: Product Behavior] If the client requests that the implementation perform a RopRestrict ([MS-OXCROPS] section 2.2.5.3) ROP request asynchronously, it does not perform the operation synchronously and not return "TBLSTAT_COMPLETE" in the TableStatus field of the ROP response buffer. (Microsoft Exchange Server 2007 follows this behavior.)</t>
   </si>
   <si>
-    <t>MS-OXCTABL_R872</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MS-OXCTABL_R915</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -6138,6 +6134,12 @@
   </si>
   <si>
     <t>[In Processing RopFindRow] If the client requested that the find be performed from a custom bookmark, as specified in section 2.2.2.1.2, but the bookmark has become invalid because of a RopResetTable ([MS-OXCROPS] section 2.2.5.15) ROP request, then the server SHOULD&lt;33&gt; set the ReturnValue field to "ecInvalidBookmark".</t>
+  </si>
+  <si>
+    <t>Verified by requirement: MS-OXCTABL_R8272.</t>
+  </si>
+  <si>
+    <t>MS-OXCTABL_R872</t>
   </si>
 </sst>
 </file>
@@ -6425,6 +6427,21 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -6448,21 +6465,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7380,7 +7382,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="6" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -7394,7 +7396,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>26</v>
@@ -7405,127 +7407,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -7538,12 +7540,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -7556,12 +7558,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -7574,12 +7576,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -7592,60 +7594,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -7737,7 +7739,7 @@
         <v>849</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="22" t="s">
@@ -7837,7 +7839,7 @@
         <v>850</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="22" t="s">
@@ -7937,7 +7939,7 @@
         <v>851</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="22" t="s">
@@ -8037,7 +8039,7 @@
         <v>852</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="D34" s="29"/>
       <c r="E34" s="29" t="s">
@@ -8112,7 +8114,7 @@
         <v>852</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="D37" s="29"/>
       <c r="E37" s="29" t="s">
@@ -8137,7 +8139,7 @@
         <v>852</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="D38" s="29"/>
       <c r="E38" s="29" t="s">
@@ -8162,7 +8164,7 @@
         <v>852</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="D39" s="29"/>
       <c r="E39" s="29" t="s">
@@ -8212,7 +8214,7 @@
         <v>853</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="D41" s="29"/>
       <c r="E41" s="29" t="s">
@@ -8237,7 +8239,7 @@
         <v>853</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="D42" s="29"/>
       <c r="E42" s="29" t="s">
@@ -8312,7 +8314,7 @@
         <v>854</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="D45" s="29"/>
       <c r="E45" s="29" t="s">
@@ -8337,7 +8339,7 @@
         <v>854</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="D46" s="29"/>
       <c r="E46" s="29" t="s">
@@ -8387,7 +8389,7 @@
         <v>855</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="D48" s="29"/>
       <c r="E48" s="29" t="s">
@@ -8412,7 +8414,7 @@
         <v>855</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="D49" s="29"/>
       <c r="E49" s="29" t="s">
@@ -9759,7 +9761,7 @@
         <v>865</v>
       </c>
       <c r="C102" s="20" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="D102" s="29"/>
       <c r="E102" s="29" t="s">
@@ -9809,7 +9811,7 @@
         <v>865</v>
       </c>
       <c r="C104" s="20" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="D104" s="29"/>
       <c r="E104" s="29" t="s">
@@ -9834,7 +9836,7 @@
         <v>865</v>
       </c>
       <c r="C105" s="20" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="D105" s="29"/>
       <c r="E105" s="29" t="s">
@@ -9909,7 +9911,7 @@
         <v>865</v>
       </c>
       <c r="C108" s="20" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="D108" s="29"/>
       <c r="E108" s="29" t="s">
@@ -9934,7 +9936,7 @@
         <v>865</v>
       </c>
       <c r="C109" s="20" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="D109" s="29"/>
       <c r="E109" s="29" t="s">
@@ -9959,7 +9961,7 @@
         <v>865</v>
       </c>
       <c r="C110" s="20" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="D110" s="29"/>
       <c r="E110" s="29" t="s">
@@ -10234,7 +10236,7 @@
         <v>865</v>
       </c>
       <c r="C121" s="20" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="D121" s="29"/>
       <c r="E121" s="29" t="s">
@@ -10259,7 +10261,7 @@
         <v>865</v>
       </c>
       <c r="C122" s="20" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="D122" s="29"/>
       <c r="E122" s="29" t="s">
@@ -10284,7 +10286,7 @@
         <v>865</v>
       </c>
       <c r="C123" s="20" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="D123" s="29"/>
       <c r="E123" s="29" t="s">
@@ -10384,7 +10386,7 @@
         <v>867</v>
       </c>
       <c r="C127" s="20" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="D127" s="29"/>
       <c r="E127" s="29" t="s">
@@ -10411,7 +10413,7 @@
         <v>867</v>
       </c>
       <c r="C128" s="20" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="D128" s="29"/>
       <c r="E128" s="29" t="s">
@@ -10436,7 +10438,7 @@
         <v>867</v>
       </c>
       <c r="C129" s="20" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="D129" s="29"/>
       <c r="E129" s="29" t="s">
@@ -10636,7 +10638,7 @@
         <v>868</v>
       </c>
       <c r="C137" s="20" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="D137" s="29"/>
       <c r="E137" s="29" t="s">
@@ -10661,7 +10663,7 @@
         <v>868</v>
       </c>
       <c r="C138" s="20" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="D138" s="29"/>
       <c r="E138" s="29" t="s">
@@ -11013,7 +11015,7 @@
         <v>871</v>
       </c>
       <c r="C152" s="20" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="D152" s="29"/>
       <c r="E152" s="29" t="s">
@@ -11038,7 +11040,7 @@
         <v>871</v>
       </c>
       <c r="C153" s="20" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="D153" s="29"/>
       <c r="E153" s="29" t="s">
@@ -11340,7 +11342,7 @@
         <v>872</v>
       </c>
       <c r="C165" s="20" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="D165" s="29"/>
       <c r="E165" s="29" t="s">
@@ -11665,7 +11667,7 @@
         <v>873</v>
       </c>
       <c r="C178" s="20" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="D178" s="29"/>
       <c r="E178" s="29" t="s">
@@ -11840,7 +11842,7 @@
         <v>875</v>
       </c>
       <c r="C185" s="20" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="D185" s="29"/>
       <c r="E185" s="29" t="s">
@@ -11892,7 +11894,7 @@
         <v>876</v>
       </c>
       <c r="C187" s="20" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="D187" s="29"/>
       <c r="E187" s="29" t="s">
@@ -12069,7 +12071,7 @@
         <v>878</v>
       </c>
       <c r="C194" s="20" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="D194" s="29"/>
       <c r="E194" s="29" t="s">
@@ -12450,7 +12452,7 @@
         <v>882</v>
       </c>
       <c r="C209" s="20" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="D209" s="29"/>
       <c r="E209" s="29" t="s">
@@ -12600,7 +12602,7 @@
         <v>883</v>
       </c>
       <c r="C215" s="20" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="D215" s="29"/>
       <c r="E215" s="29" t="s">
@@ -12625,7 +12627,7 @@
         <v>883</v>
       </c>
       <c r="C216" s="20" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="D216" s="29"/>
       <c r="E216" s="29" t="s">
@@ -12650,7 +12652,7 @@
         <v>883</v>
       </c>
       <c r="C217" s="20" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="D217" s="29"/>
       <c r="E217" s="29" t="s">
@@ -13179,7 +13181,7 @@
         <v>885</v>
       </c>
       <c r="C238" s="20" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="D238" s="29"/>
       <c r="E238" s="29" t="s">
@@ -13204,7 +13206,7 @@
         <v>885</v>
       </c>
       <c r="C239" s="20" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="D239" s="29"/>
       <c r="E239" s="29" t="s">
@@ -13354,7 +13356,7 @@
         <v>886</v>
       </c>
       <c r="C245" s="20" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="D245" s="29"/>
       <c r="E245" s="29" t="s">
@@ -13404,7 +13406,7 @@
         <v>886</v>
       </c>
       <c r="C247" s="20" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="D247" s="29"/>
       <c r="E247" s="29" t="s">
@@ -13429,7 +13431,7 @@
         <v>886</v>
       </c>
       <c r="C248" s="20" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="D248" s="29"/>
       <c r="E248" s="29" t="s">
@@ -13454,7 +13456,7 @@
         <v>886</v>
       </c>
       <c r="C249" s="20" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="D249" s="29"/>
       <c r="E249" s="29" t="s">
@@ -13631,7 +13633,7 @@
         <v>887</v>
       </c>
       <c r="C256" s="20" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="D256" s="29"/>
       <c r="E256" s="29" t="s">
@@ -13656,7 +13658,7 @@
         <v>887</v>
       </c>
       <c r="C257" s="20" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="D257" s="29"/>
       <c r="E257" s="29" t="s">
@@ -13706,7 +13708,7 @@
         <v>887</v>
       </c>
       <c r="C259" s="20" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="D259" s="29"/>
       <c r="E259" s="29" t="s">
@@ -13731,7 +13733,7 @@
         <v>887</v>
       </c>
       <c r="C260" s="20" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="D260" s="29"/>
       <c r="E260" s="29" t="s">
@@ -13981,7 +13983,7 @@
         <v>888</v>
       </c>
       <c r="C270" s="20" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="D270" s="29"/>
       <c r="E270" s="29" t="s">
@@ -14335,7 +14337,7 @@
         <v>891</v>
       </c>
       <c r="C284" s="20" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="D284" s="29"/>
       <c r="E284" s="29" t="s">
@@ -14562,7 +14564,7 @@
         <v>893</v>
       </c>
       <c r="C293" s="20" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="D293" s="29"/>
       <c r="E293" s="29" t="s">
@@ -14939,7 +14941,7 @@
         <v>897</v>
       </c>
       <c r="C308" s="20" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="D308" s="29"/>
       <c r="E308" s="29" t="s">
@@ -15189,7 +15191,7 @@
         <v>898</v>
       </c>
       <c r="C318" s="20" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="D318" s="29"/>
       <c r="E318" s="29" t="s">
@@ -15214,7 +15216,7 @@
         <v>898</v>
       </c>
       <c r="C319" s="20" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="D319" s="29"/>
       <c r="E319" s="29" t="s">
@@ -15264,7 +15266,7 @@
         <v>899</v>
       </c>
       <c r="C321" s="20" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="D321" s="29"/>
       <c r="E321" s="29" t="s">
@@ -15289,7 +15291,7 @@
         <v>899</v>
       </c>
       <c r="C322" s="20" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="D322" s="29"/>
       <c r="E322" s="29" t="s">
@@ -15305,7 +15307,7 @@
         <v>17</v>
       </c>
       <c r="I322" s="20" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="323" spans="1:9" ht="45">
@@ -15341,7 +15343,7 @@
         <v>899</v>
       </c>
       <c r="C324" s="20" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="D324" s="29"/>
       <c r="E324" s="29" t="s">
@@ -15366,7 +15368,7 @@
         <v>899</v>
       </c>
       <c r="C325" s="20" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="D325" s="29"/>
       <c r="E325" s="29" t="s">
@@ -15391,7 +15393,7 @@
         <v>899</v>
       </c>
       <c r="C326" s="20" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="D326" s="29"/>
       <c r="E326" s="29" t="s">
@@ -15416,7 +15418,7 @@
         <v>899</v>
       </c>
       <c r="C327" s="20" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="D327" s="29"/>
       <c r="E327" s="29" t="s">
@@ -15516,7 +15518,7 @@
         <v>900</v>
       </c>
       <c r="C331" s="20" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="D331" s="29"/>
       <c r="E331" s="29" t="s">
@@ -15537,13 +15539,13 @@
     </row>
     <row r="332" spans="1:9" ht="30">
       <c r="A332" s="22" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="B332" s="24" t="s">
         <v>900</v>
       </c>
       <c r="C332" s="20" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="D332" s="33"/>
       <c r="E332" s="29" t="s">
@@ -15568,7 +15570,7 @@
         <v>900</v>
       </c>
       <c r="C333" s="20" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="D333" s="29"/>
       <c r="E333" s="29" t="s">
@@ -15718,7 +15720,7 @@
         <v>901</v>
       </c>
       <c r="C339" s="20" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="D339" s="29"/>
       <c r="E339" s="29" t="s">
@@ -15743,7 +15745,7 @@
         <v>901</v>
       </c>
       <c r="C340" s="20" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="D340" s="29"/>
       <c r="E340" s="29" t="s">
@@ -15768,7 +15770,7 @@
         <v>901</v>
       </c>
       <c r="C341" s="20" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="D341" s="29"/>
       <c r="E341" s="29" t="s">
@@ -15843,7 +15845,7 @@
         <v>903</v>
       </c>
       <c r="C344" s="20" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="D344" s="29"/>
       <c r="E344" s="29" t="s">
@@ -15868,7 +15870,7 @@
         <v>903</v>
       </c>
       <c r="C345" s="20" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="D345" s="29"/>
       <c r="E345" s="29" t="s">
@@ -15972,7 +15974,7 @@
         <v>903</v>
       </c>
       <c r="C349" s="20" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="D349" s="29"/>
       <c r="E349" s="29" t="s">
@@ -16197,7 +16199,7 @@
         <v>906</v>
       </c>
       <c r="C358" s="20" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="D358" s="29"/>
       <c r="E358" s="29" t="s">
@@ -16376,7 +16378,7 @@
         <v>907</v>
       </c>
       <c r="C365" s="20" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
       <c r="D365" s="29"/>
       <c r="E365" s="29" t="s">
@@ -16401,7 +16403,7 @@
         <v>907</v>
       </c>
       <c r="C366" s="20" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="D366" s="29"/>
       <c r="E366" s="29" t="s">
@@ -16426,7 +16428,7 @@
         <v>907</v>
       </c>
       <c r="C367" s="20" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="D367" s="29"/>
       <c r="E367" s="29" t="s">
@@ -16476,7 +16478,7 @@
         <v>908</v>
       </c>
       <c r="C369" s="20" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="D369" s="29"/>
       <c r="E369" s="29" t="s">
@@ -16576,7 +16578,7 @@
         <v>909</v>
       </c>
       <c r="C373" s="20" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="D373" s="29"/>
       <c r="E373" s="29" t="s">
@@ -16703,7 +16705,7 @@
         <v>910</v>
       </c>
       <c r="C378" s="20" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="D378" s="29"/>
       <c r="E378" s="29" t="s">
@@ -16728,7 +16730,7 @@
         <v>910</v>
       </c>
       <c r="C379" s="20" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="D379" s="29"/>
       <c r="E379" s="29" t="s">
@@ -17205,7 +17207,7 @@
         <v>915</v>
       </c>
       <c r="C398" s="20" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="D398" s="29"/>
       <c r="E398" s="29" t="s">
@@ -17255,7 +17257,7 @@
         <v>915</v>
       </c>
       <c r="C400" s="20" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="D400" s="29"/>
       <c r="E400" s="29" t="s">
@@ -17480,7 +17482,7 @@
         <v>917</v>
       </c>
       <c r="C409" s="20" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="D409" s="29"/>
       <c r="E409" s="29" t="s">
@@ -17680,7 +17682,7 @@
         <v>919</v>
       </c>
       <c r="C417" s="20" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="D417" s="29"/>
       <c r="E417" s="29" t="s">
@@ -17780,7 +17782,7 @@
         <v>919</v>
       </c>
       <c r="C421" s="20" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="D421" s="29"/>
       <c r="E421" s="29" t="s">
@@ -17830,7 +17832,7 @@
         <v>919</v>
       </c>
       <c r="C423" s="20" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="D423" s="29"/>
       <c r="E423" s="29" t="s">
@@ -17855,7 +17857,7 @@
         <v>919</v>
       </c>
       <c r="C424" s="20" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="D424" s="29"/>
       <c r="E424" s="29" t="s">
@@ -17905,7 +17907,7 @@
         <v>919</v>
       </c>
       <c r="C426" s="20" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="D426" s="29"/>
       <c r="E426" s="29" t="s">
@@ -18130,7 +18132,7 @@
         <v>32</v>
       </c>
       <c r="C435" s="20" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="D435" s="29"/>
       <c r="E435" s="29" t="s">
@@ -18280,7 +18282,7 @@
         <v>921</v>
       </c>
       <c r="C441" s="20" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="D441" s="29"/>
       <c r="E441" s="29" t="s">
@@ -18330,7 +18332,7 @@
         <v>921</v>
       </c>
       <c r="C443" s="20" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="D443" s="29"/>
       <c r="E443" s="29" t="s">
@@ -18530,7 +18532,7 @@
         <v>921</v>
       </c>
       <c r="C451" s="20" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="D451" s="29"/>
       <c r="E451" s="29" t="s">
@@ -18630,7 +18632,7 @@
         <v>33</v>
       </c>
       <c r="C455" s="20" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="D455" s="29"/>
       <c r="E455" s="29" t="s">
@@ -18655,7 +18657,7 @@
         <v>33</v>
       </c>
       <c r="C456" s="20" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="D456" s="29"/>
       <c r="E456" s="29" t="s">
@@ -18705,7 +18707,7 @@
         <v>33</v>
       </c>
       <c r="C458" s="20" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="D458" s="29"/>
       <c r="E458" s="29" t="s">
@@ -18755,7 +18757,7 @@
         <v>922</v>
       </c>
       <c r="C460" s="20" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="D460" s="29"/>
       <c r="E460" s="29" t="s">
@@ -18905,7 +18907,7 @@
         <v>922</v>
       </c>
       <c r="C466" s="20" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="D466" s="29"/>
       <c r="E466" s="29" t="s">
@@ -18980,7 +18982,7 @@
         <v>922</v>
       </c>
       <c r="C469" s="20" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="D469" s="29"/>
       <c r="E469" s="29" t="s">
@@ -19005,7 +19007,7 @@
         <v>923</v>
       </c>
       <c r="C470" s="20" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="D470" s="29"/>
       <c r="E470" s="29" t="s">
@@ -19030,7 +19032,7 @@
         <v>923</v>
       </c>
       <c r="C471" s="20" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="D471" s="29"/>
       <c r="E471" s="29" t="s">
@@ -19055,7 +19057,7 @@
         <v>923</v>
       </c>
       <c r="C472" s="20" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="D472" s="29"/>
       <c r="E472" s="29" t="s">
@@ -19480,7 +19482,7 @@
         <v>926</v>
       </c>
       <c r="C489" s="20" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="D489" s="29"/>
       <c r="E489" s="29" t="s">
@@ -19782,7 +19784,7 @@
         <v>930</v>
       </c>
       <c r="C501" s="20" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
       <c r="D501" s="29"/>
       <c r="E501" s="29" t="s">
@@ -19809,7 +19811,7 @@
         <v>930</v>
       </c>
       <c r="C502" s="20" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="D502" s="29"/>
       <c r="E502" s="29" t="s">
@@ -19836,7 +19838,7 @@
         <v>930</v>
       </c>
       <c r="C503" s="20" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="D503" s="29"/>
       <c r="E503" s="29" t="s">
@@ -19863,7 +19865,7 @@
         <v>930</v>
       </c>
       <c r="C504" s="20" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="D504" s="29"/>
       <c r="E504" s="29" t="s">
@@ -19915,7 +19917,7 @@
         <v>930</v>
       </c>
       <c r="C506" s="20" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="D506" s="29"/>
       <c r="E506" s="29" t="s">
@@ -19990,7 +19992,7 @@
         <v>930</v>
       </c>
       <c r="C509" s="20" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="D509" s="29"/>
       <c r="E509" s="29" t="s">
@@ -20015,7 +20017,7 @@
         <v>930</v>
       </c>
       <c r="C510" s="20" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="D510" s="29"/>
       <c r="E510" s="29" t="s">
@@ -20165,7 +20167,7 @@
         <v>931</v>
       </c>
       <c r="C516" s="20" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="D516" s="29"/>
       <c r="E516" s="29" t="s">
@@ -20192,7 +20194,7 @@
         <v>931</v>
       </c>
       <c r="C517" s="20" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="D517" s="29"/>
       <c r="E517" s="29" t="s">
@@ -20213,13 +20215,13 @@
     </row>
     <row r="518" spans="1:9" ht="45">
       <c r="A518" s="22" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="B518" s="34" t="s">
         <v>931</v>
       </c>
       <c r="C518" s="20" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="D518" s="33"/>
       <c r="E518" s="29" t="s">
@@ -20235,18 +20237,18 @@
         <v>17</v>
       </c>
       <c r="I518" s="20" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="519" spans="1:9" ht="45">
       <c r="A519" s="22" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="B519" s="34" t="s">
         <v>931</v>
       </c>
       <c r="C519" s="20" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="D519" s="33"/>
       <c r="E519" s="29" t="s">
@@ -20262,18 +20264,18 @@
         <v>17</v>
       </c>
       <c r="I519" s="20" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="520" spans="1:9" ht="45">
       <c r="A520" s="22" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="B520" s="34" t="s">
         <v>931</v>
       </c>
       <c r="C520" s="20" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="D520" s="33"/>
       <c r="E520" s="29" t="s">
@@ -20289,18 +20291,18 @@
         <v>17</v>
       </c>
       <c r="I520" s="20" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="521" spans="1:9" ht="45">
       <c r="A521" s="22" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="B521" s="34" t="s">
         <v>931</v>
       </c>
       <c r="C521" s="20" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
       <c r="D521" s="33"/>
       <c r="E521" s="29" t="s">
@@ -20316,18 +20318,18 @@
         <v>17</v>
       </c>
       <c r="I521" s="20" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="522" spans="1:9" ht="45">
       <c r="A522" s="22" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="B522" s="34" t="s">
         <v>931</v>
       </c>
       <c r="C522" s="20" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="D522" s="33"/>
       <c r="E522" s="29" t="s">
@@ -20343,18 +20345,18 @@
         <v>17</v>
       </c>
       <c r="I522" s="20" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="523" spans="1:9" ht="45">
       <c r="A523" s="22" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="B523" s="34" t="s">
         <v>931</v>
       </c>
       <c r="C523" s="20" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
       <c r="D523" s="33"/>
       <c r="E523" s="29" t="s">
@@ -20370,18 +20372,18 @@
         <v>17</v>
       </c>
       <c r="I523" s="20" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="524" spans="1:9" ht="45">
       <c r="A524" s="22" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="B524" s="34" t="s">
         <v>931</v>
       </c>
       <c r="C524" s="20" t="s">
-        <v>1811</v>
+        <v>1810</v>
       </c>
       <c r="D524" s="33"/>
       <c r="E524" s="29" t="s">
@@ -20397,7 +20399,7 @@
         <v>17</v>
       </c>
       <c r="I524" s="20" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="525" spans="1:9" ht="45">
@@ -20460,7 +20462,7 @@
         <v>931</v>
       </c>
       <c r="C527" s="20" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="D527" s="29"/>
       <c r="E527" s="29" t="s">
@@ -20793,7 +20795,7 @@
         <v>932</v>
       </c>
       <c r="C540" s="20" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
       <c r="D540" s="29"/>
       <c r="E540" s="29" t="s">
@@ -20922,7 +20924,7 @@
         <v>932</v>
       </c>
       <c r="C545" s="20" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="D545" s="29"/>
       <c r="E545" s="29" t="s">
@@ -21074,7 +21076,7 @@
         <v>933</v>
       </c>
       <c r="C551" s="20" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="D551" s="29"/>
       <c r="E551" s="29" t="s">
@@ -21099,7 +21101,7 @@
         <v>933</v>
       </c>
       <c r="C552" s="20" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="D552" s="29"/>
       <c r="E552" s="29" t="s">
@@ -21124,7 +21126,7 @@
         <v>933</v>
       </c>
       <c r="C553" s="20" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="D553" s="29"/>
       <c r="E553" s="29" t="s">
@@ -21149,7 +21151,7 @@
         <v>933</v>
       </c>
       <c r="C554" s="20" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="D554" s="29"/>
       <c r="E554" s="29" t="s">
@@ -21174,7 +21176,7 @@
         <v>933</v>
       </c>
       <c r="C555" s="20" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="D555" s="29"/>
       <c r="E555" s="29" t="s">
@@ -21201,7 +21203,7 @@
         <v>933</v>
       </c>
       <c r="C556" s="20" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="D556" s="29"/>
       <c r="E556" s="29" t="s">
@@ -21226,7 +21228,7 @@
         <v>933</v>
       </c>
       <c r="C557" s="20" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="D557" s="29"/>
       <c r="E557" s="29" t="s">
@@ -21247,13 +21249,13 @@
     </row>
     <row r="558" spans="1:9" ht="30">
       <c r="A558" s="29" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="B558" s="30" t="s">
         <v>933</v>
       </c>
       <c r="C558" s="31" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="D558" s="29"/>
       <c r="E558" s="29" t="s">
@@ -21281,7 +21283,7 @@
         <v>1365</v>
       </c>
       <c r="D559" s="29" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
       <c r="E559" s="29" t="s">
         <v>19</v>
@@ -21434,7 +21436,7 @@
         <v>933</v>
       </c>
       <c r="C565" s="20" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="D565" s="29"/>
       <c r="E565" s="29" t="s">
@@ -21661,7 +21663,7 @@
         <v>934</v>
       </c>
       <c r="C574" s="20" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="D574" s="29"/>
       <c r="E574" s="29" t="s">
@@ -22402,7 +22404,7 @@
         <v>936</v>
       </c>
       <c r="C603" s="20" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="D603" s="29"/>
       <c r="E603" s="29" t="s">
@@ -22891,7 +22893,7 @@
         <v>938</v>
       </c>
       <c r="C622" s="20" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="D622" s="29"/>
       <c r="E622" s="29" t="s">
@@ -23147,7 +23149,7 @@
         <v>939</v>
       </c>
       <c r="C632" s="20" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
       <c r="D632" s="29"/>
       <c r="E632" s="29" t="s">
@@ -23172,7 +23174,7 @@
         <v>939</v>
       </c>
       <c r="C633" s="20" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="D633" s="29"/>
       <c r="E633" s="29" t="s">
@@ -23199,7 +23201,7 @@
         <v>939</v>
       </c>
       <c r="C634" s="20" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
       <c r="D634" s="29"/>
       <c r="E634" s="29" t="s">
@@ -23215,7 +23217,7 @@
         <v>17</v>
       </c>
       <c r="I634" s="20" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="635" spans="1:9" ht="45">
@@ -23226,7 +23228,7 @@
         <v>939</v>
       </c>
       <c r="C635" s="20" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="D635" s="29"/>
       <c r="E635" s="29" t="s">
@@ -23242,7 +23244,7 @@
         <v>17</v>
       </c>
       <c r="I635" s="20" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
     </row>
     <row r="636" spans="1:9" ht="60">
@@ -23253,7 +23255,7 @@
         <v>939</v>
       </c>
       <c r="C636" s="20" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="D636" s="29"/>
       <c r="E636" s="29" t="s">
@@ -23457,7 +23459,7 @@
         <v>939</v>
       </c>
       <c r="C644" s="20" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="D644" s="29"/>
       <c r="E644" s="29" t="s">
@@ -23507,7 +23509,7 @@
         <v>940</v>
       </c>
       <c r="C646" s="20" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
       <c r="D646" s="29"/>
       <c r="E646" s="29" t="s">
@@ -23632,7 +23634,7 @@
         <v>940</v>
       </c>
       <c r="C651" s="20" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="D651" s="29"/>
       <c r="E651" s="29" t="s">
@@ -23838,7 +23840,7 @@
         <v>941</v>
       </c>
       <c r="C659" s="20" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="D659" s="29"/>
       <c r="E659" s="29" t="s">
@@ -23863,7 +23865,7 @@
         <v>941</v>
       </c>
       <c r="C660" s="20" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
       <c r="D660" s="29"/>
       <c r="E660" s="29" t="s">
@@ -23888,7 +23890,7 @@
         <v>941</v>
       </c>
       <c r="C661" s="20" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
       <c r="D661" s="29"/>
       <c r="E661" s="29" t="s">
@@ -23913,7 +23915,7 @@
         <v>941</v>
       </c>
       <c r="C662" s="20" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="D662" s="29"/>
       <c r="E662" s="29" t="s">
@@ -23938,7 +23940,7 @@
         <v>941</v>
       </c>
       <c r="C663" s="20" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="D663" s="29"/>
       <c r="E663" s="29" t="s">
@@ -23963,7 +23965,7 @@
         <v>941</v>
       </c>
       <c r="C664" s="20" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="D664" s="29"/>
       <c r="E664" s="29" t="s">
@@ -23988,7 +23990,7 @@
         <v>941</v>
       </c>
       <c r="C665" s="20" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="D665" s="29"/>
       <c r="E665" s="29" t="s">
@@ -24013,7 +24015,7 @@
         <v>941</v>
       </c>
       <c r="C666" s="20" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
       <c r="D666" s="29"/>
       <c r="E666" s="29" t="s">
@@ -24423,7 +24425,7 @@
         <v>943</v>
       </c>
       <c r="C682" s="20" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="D682" s="29"/>
       <c r="E682" s="29" t="s">
@@ -24498,7 +24500,7 @@
         <v>943</v>
       </c>
       <c r="C685" s="20" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="D685" s="29"/>
       <c r="E685" s="29" t="s">
@@ -24525,7 +24527,7 @@
         <v>943</v>
       </c>
       <c r="C686" s="20" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="D686" s="29"/>
       <c r="E686" s="29" t="s">
@@ -24541,7 +24543,7 @@
         <v>17</v>
       </c>
       <c r="I686" s="20" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
     </row>
     <row r="687" spans="1:9" ht="60">
@@ -24552,7 +24554,7 @@
         <v>943</v>
       </c>
       <c r="C687" s="20" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="D687" s="29"/>
       <c r="E687" s="29" t="s">
@@ -24579,7 +24581,7 @@
         <v>943</v>
       </c>
       <c r="C688" s="20" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="D688" s="29"/>
       <c r="E688" s="29" t="s">
@@ -24654,7 +24656,7 @@
         <v>943</v>
       </c>
       <c r="C691" s="20" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="D691" s="29"/>
       <c r="E691" s="29" t="s">
@@ -24860,7 +24862,7 @@
         <v>944</v>
       </c>
       <c r="C699" s="20" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
       <c r="D699" s="29"/>
       <c r="E699" s="29" t="s">
@@ -24885,7 +24887,7 @@
         <v>944</v>
       </c>
       <c r="C700" s="20" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="D700" s="29"/>
       <c r="E700" s="29" t="s">
@@ -24935,7 +24937,7 @@
         <v>944</v>
       </c>
       <c r="C702" s="20" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="D702" s="29"/>
       <c r="E702" s="29" t="s">
@@ -25037,7 +25039,7 @@
         <v>944</v>
       </c>
       <c r="C706" s="20" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="D706" s="29"/>
       <c r="E706" s="29" t="s">
@@ -25056,13 +25058,13 @@
     </row>
     <row r="707" spans="1:9" ht="45">
       <c r="A707" s="22" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="B707" s="24" t="s">
         <v>944</v>
       </c>
       <c r="C707" s="20" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
       <c r="D707" s="33"/>
       <c r="E707" s="29" t="s">
@@ -25137,7 +25139,7 @@
         <v>945</v>
       </c>
       <c r="C710" s="20" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="D710" s="29"/>
       <c r="E710" s="29" t="s">
@@ -25162,7 +25164,7 @@
         <v>945</v>
       </c>
       <c r="C711" s="20" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="D711" s="29"/>
       <c r="E711" s="29" t="s">
@@ -25312,7 +25314,7 @@
         <v>945</v>
       </c>
       <c r="C717" s="20" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="D717" s="29"/>
       <c r="E717" s="29" t="s">
@@ -25337,7 +25339,7 @@
         <v>945</v>
       </c>
       <c r="C718" s="20" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="D718" s="29"/>
       <c r="E718" s="29" t="s">
@@ -25587,7 +25589,7 @@
         <v>946</v>
       </c>
       <c r="C728" s="20" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="D728" s="29"/>
       <c r="E728" s="29" t="s">
@@ -25837,7 +25839,7 @@
         <v>948</v>
       </c>
       <c r="C738" s="20" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="D738" s="29"/>
       <c r="E738" s="29" t="s">
@@ -25862,7 +25864,7 @@
         <v>948</v>
       </c>
       <c r="C739" s="20" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="D739" s="29"/>
       <c r="E739" s="29" t="s">
@@ -26012,7 +26014,7 @@
         <v>949</v>
       </c>
       <c r="C745" s="20" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="D745" s="29"/>
       <c r="E745" s="29" t="s">
@@ -26037,7 +26039,7 @@
         <v>949</v>
       </c>
       <c r="C746" s="20" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="D746" s="29"/>
       <c r="E746" s="29" t="s">
@@ -26212,7 +26214,7 @@
         <v>950</v>
       </c>
       <c r="C753" s="20" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="D753" s="22" t="s">
         <v>1535</v>
@@ -26326,7 +26328,7 @@
         <v>950</v>
       </c>
       <c r="C757" s="20" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="D757" s="29" t="s">
         <v>1538</v>
@@ -26411,7 +26413,7 @@
         <v>950</v>
       </c>
       <c r="C760" s="20" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="D760" s="29"/>
       <c r="E760" s="29" t="s">
@@ -26438,7 +26440,7 @@
         <v>950</v>
       </c>
       <c r="C761" s="20" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="D761" s="29" t="s">
         <v>1532</v>
@@ -26467,7 +26469,7 @@
         <v>950</v>
       </c>
       <c r="C762" s="20" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
       <c r="D762" s="29"/>
       <c r="E762" s="29" t="s">
@@ -26494,7 +26496,7 @@
         <v>950</v>
       </c>
       <c r="C763" s="20" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
       <c r="D763" s="29"/>
       <c r="E763" s="29" t="s">
@@ -26521,7 +26523,7 @@
         <v>950</v>
       </c>
       <c r="C764" s="20" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="D764" s="29" t="s">
         <v>1533</v>
@@ -26550,7 +26552,7 @@
         <v>950</v>
       </c>
       <c r="C765" s="20" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="D765" s="29"/>
       <c r="E765" s="29" t="s">
@@ -26577,7 +26579,7 @@
         <v>950</v>
       </c>
       <c r="C766" s="20" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="D766" s="29"/>
       <c r="E766" s="29" t="s">
@@ -26604,7 +26606,7 @@
         <v>950</v>
       </c>
       <c r="C767" s="20" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="D767" s="29" t="s">
         <v>1534</v>
@@ -26633,7 +26635,7 @@
         <v>950</v>
       </c>
       <c r="C768" s="20" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="D768" s="29"/>
       <c r="E768" s="29" t="s">
@@ -26654,13 +26656,13 @@
     </row>
     <row r="769" spans="1:9" ht="45">
       <c r="A769" s="22" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="B769" s="24" t="s">
         <v>950</v>
       </c>
       <c r="C769" s="20" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="D769" s="33"/>
       <c r="E769" s="33" t="s">
@@ -26685,7 +26687,7 @@
         <v>950</v>
       </c>
       <c r="C770" s="20" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="D770" s="29"/>
       <c r="E770" s="29" t="s">
@@ -26710,7 +26712,7 @@
         <v>950</v>
       </c>
       <c r="C771" s="20" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
       <c r="D771" s="22" t="s">
         <v>1540</v>
@@ -26766,7 +26768,7 @@
         <v>950</v>
       </c>
       <c r="C773" s="20" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="D773" s="29"/>
       <c r="E773" s="29" t="s">
@@ -26791,7 +26793,7 @@
         <v>950</v>
       </c>
       <c r="C774" s="20" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="D774" s="29" t="s">
         <v>1541</v>
@@ -26847,7 +26849,7 @@
         <v>950</v>
       </c>
       <c r="C776" s="20" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="D776" s="29"/>
       <c r="E776" s="29" t="s">
@@ -26872,7 +26874,7 @@
         <v>950</v>
       </c>
       <c r="C777" s="20" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="D777" s="29"/>
       <c r="E777" s="29" t="s">
@@ -26899,10 +26901,10 @@
         <v>950</v>
       </c>
       <c r="C778" s="20" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="D778" s="22" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="E778" s="29" t="s">
         <v>22</v>
@@ -26922,16 +26924,16 @@
     </row>
     <row r="779" spans="1:9" ht="45">
       <c r="A779" s="22" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="B779" s="24" t="s">
         <v>950</v>
       </c>
       <c r="C779" s="20" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="D779" s="22" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="E779" s="29" t="s">
         <v>22</v>
@@ -26957,7 +26959,7 @@
         <v>950</v>
       </c>
       <c r="C780" s="20" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
       <c r="D780" s="29"/>
       <c r="E780" s="29" t="s">
@@ -26984,7 +26986,7 @@
         <v>950</v>
       </c>
       <c r="C781" s="20" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="D781" s="29"/>
       <c r="E781" s="29" t="s">
@@ -27009,7 +27011,7 @@
         <v>950</v>
       </c>
       <c r="C782" s="20" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="D782" s="29"/>
       <c r="E782" s="29" t="s">
@@ -27036,7 +27038,7 @@
         <v>950</v>
       </c>
       <c r="C783" s="20" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="D783" s="29"/>
       <c r="E783" s="29" t="s">
@@ -27061,7 +27063,7 @@
         <v>950</v>
       </c>
       <c r="C784" s="20" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
       <c r="D784" s="29"/>
       <c r="E784" s="29" t="s">
@@ -27088,7 +27090,7 @@
         <v>950</v>
       </c>
       <c r="C785" s="20" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
       <c r="D785" s="29"/>
       <c r="E785" s="29" t="s">
@@ -27115,7 +27117,7 @@
         <v>950</v>
       </c>
       <c r="C786" s="20" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="D786" s="29" t="s">
         <v>1542</v>
@@ -27202,7 +27204,7 @@
         <v>950</v>
       </c>
       <c r="C789" s="20" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="D789" s="29" t="s">
         <v>1543</v>
@@ -27260,7 +27262,7 @@
         <v>950</v>
       </c>
       <c r="C791" s="20" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="D791" s="29" t="s">
         <v>1544</v>
@@ -27283,13 +27285,13 @@
     </row>
     <row r="792" spans="1:9" ht="60">
       <c r="A792" s="22" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="B792" s="30" t="s">
         <v>950</v>
       </c>
       <c r="C792" s="20" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="D792" s="29" t="s">
         <v>1546</v>
@@ -27368,16 +27370,16 @@
     </row>
     <row r="795" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A795" s="22" t="s">
-        <v>1921</v>
+        <v>1920</v>
       </c>
       <c r="B795" s="24" t="s">
         <v>950</v>
       </c>
       <c r="C795" s="20" t="s">
+        <v>1927</v>
+      </c>
+      <c r="D795" s="22" t="s">
         <v>1928</v>
-      </c>
-      <c r="D795" s="22" t="s">
-        <v>1929</v>
       </c>
       <c r="E795" s="29" t="s">
         <v>22</v>
@@ -27397,16 +27399,16 @@
     </row>
     <row r="796" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A796" s="22" t="s">
-        <v>1922</v>
+        <v>1921</v>
       </c>
       <c r="B796" s="24" t="s">
         <v>950</v>
       </c>
       <c r="C796" s="20" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D796" s="22" t="s">
         <v>1930</v>
-      </c>
-      <c r="D796" s="22" t="s">
-        <v>1931</v>
       </c>
       <c r="E796" s="29" t="s">
         <v>22</v>
@@ -27424,16 +27426,16 @@
     </row>
     <row r="797" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A797" s="22" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
       <c r="B797" s="24" t="s">
         <v>950</v>
       </c>
       <c r="C797" s="20" t="s">
+        <v>1931</v>
+      </c>
+      <c r="D797" s="22" t="s">
         <v>1932</v>
-      </c>
-      <c r="D797" s="22" t="s">
-        <v>1933</v>
       </c>
       <c r="E797" s="29" t="s">
         <v>22</v>
@@ -27453,16 +27455,16 @@
     </row>
     <row r="798" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A798" s="22" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
       <c r="B798" s="24" t="s">
         <v>950</v>
       </c>
       <c r="C798" s="20" t="s">
+        <v>1933</v>
+      </c>
+      <c r="D798" s="22" t="s">
         <v>1934</v>
-      </c>
-      <c r="D798" s="22" t="s">
-        <v>1935</v>
       </c>
       <c r="E798" s="29" t="s">
         <v>22</v>
@@ -27482,16 +27484,16 @@
     </row>
     <row r="799" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A799" s="22" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
       <c r="B799" s="24" t="s">
         <v>950</v>
       </c>
       <c r="C799" s="20" t="s">
+        <v>1935</v>
+      </c>
+      <c r="D799" s="22" t="s">
         <v>1936</v>
-      </c>
-      <c r="D799" s="22" t="s">
-        <v>1937</v>
       </c>
       <c r="E799" s="29" t="s">
         <v>22</v>
@@ -27511,16 +27513,16 @@
     </row>
     <row r="800" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A800" s="22" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="B800" s="24" t="s">
         <v>950</v>
       </c>
       <c r="C800" s="20" t="s">
+        <v>1937</v>
+      </c>
+      <c r="D800" s="22" t="s">
         <v>1938</v>
-      </c>
-      <c r="D800" s="22" t="s">
-        <v>1939</v>
       </c>
       <c r="E800" s="29" t="s">
         <v>22</v>
@@ -27540,16 +27542,16 @@
     </row>
     <row r="801" spans="1:9" s="36" customFormat="1" ht="45">
       <c r="A801" s="22" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="B801" s="24" t="s">
         <v>950</v>
       </c>
       <c r="C801" s="20" t="s">
+        <v>1939</v>
+      </c>
+      <c r="D801" s="22" t="s">
         <v>1940</v>
-      </c>
-      <c r="D801" s="22" t="s">
-        <v>1941</v>
       </c>
       <c r="E801" s="29" t="s">
         <v>22</v>
@@ -27575,7 +27577,7 @@
         <v>950</v>
       </c>
       <c r="C802" s="20" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="D802" s="29" t="s">
         <v>1549</v>
@@ -27631,7 +27633,7 @@
         <v>950</v>
       </c>
       <c r="C804" s="20" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="D804" s="29" t="s">
         <v>1551</v>
@@ -27687,7 +27689,7 @@
         <v>950</v>
       </c>
       <c r="C806" s="20" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="D806" s="29" t="s">
         <v>1553</v>
@@ -27774,7 +27776,7 @@
         <v>950</v>
       </c>
       <c r="C809" s="20" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="D809" s="29" t="s">
         <v>1556</v>
@@ -27803,7 +27805,7 @@
         <v>950</v>
       </c>
       <c r="C810" s="20" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
       <c r="D810" s="29" t="s">
         <v>1557</v>
@@ -27857,7 +27859,7 @@
         <v>950</v>
       </c>
       <c r="C812" s="20" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="D812" s="29"/>
       <c r="E812" s="29" t="s">
@@ -27882,7 +27884,7 @@
         <v>950</v>
       </c>
       <c r="C813" s="20" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="D813" s="22" t="s">
         <v>1559</v>
@@ -27911,7 +27913,7 @@
         <v>950</v>
       </c>
       <c r="C814" s="20" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="D814" s="29" t="s">
         <v>1559</v>
@@ -27940,7 +27942,7 @@
         <v>950</v>
       </c>
       <c r="C815" s="20" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="D815" s="29" t="s">
         <v>1560</v>
@@ -27963,13 +27965,13 @@
     </row>
     <row r="816" spans="1:9" ht="60">
       <c r="A816" s="22" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="B816" s="30" t="s">
         <v>950</v>
       </c>
       <c r="C816" s="20" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="D816" s="29" t="s">
         <v>1560</v>
@@ -27996,7 +27998,7 @@
         <v>950</v>
       </c>
       <c r="C817" s="20" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="D817" s="29" t="s">
         <v>1561</v>
@@ -28023,7 +28025,7 @@
         <v>950</v>
       </c>
       <c r="C818" s="20" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="D818" s="29" t="s">
         <v>1561</v>
@@ -28052,7 +28054,7 @@
         <v>950</v>
       </c>
       <c r="C819" s="20" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="D819" s="29"/>
       <c r="E819" s="29" t="s">
@@ -28077,7 +28079,7 @@
         <v>950</v>
       </c>
       <c r="C820" s="20" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="D820" s="29"/>
       <c r="E820" s="29" t="s">
@@ -28092,7 +28094,7 @@
       <c r="H820" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="I820" s="31" t="s">
+      <c r="I820" s="20" t="s">
         <v>1651</v>
       </c>
     </row>
@@ -28104,7 +28106,7 @@
         <v>950</v>
       </c>
       <c r="C821" s="20" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
       <c r="D821" s="29"/>
       <c r="E821" s="29" t="s">
@@ -28123,13 +28125,13 @@
     </row>
     <row r="822" spans="1:9" ht="75">
       <c r="A822" s="22" t="s">
+        <v>1667</v>
+      </c>
+      <c r="B822" s="30" t="s">
         <v>1668</v>
       </c>
-      <c r="B822" s="30" t="s">
-        <v>1669</v>
-      </c>
       <c r="C822" s="20" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
       <c r="D822" s="29"/>
       <c r="E822" s="29" t="s">
@@ -28148,13 +28150,13 @@
     </row>
     <row r="823" spans="1:9" ht="75">
       <c r="A823" s="22" t="s">
-        <v>1667</v>
+        <v>1957</v>
       </c>
       <c r="B823" s="30" t="s">
         <v>950</v>
       </c>
       <c r="C823" s="20" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
       <c r="D823" s="29"/>
       <c r="E823" s="29" t="s">
@@ -28167,21 +28169,19 @@
         <v>15</v>
       </c>
       <c r="H823" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I823" s="31" t="s">
-        <v>1593</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I823" s="31"/>
     </row>
     <row r="824" spans="1:9" ht="45">
       <c r="A824" s="22" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="B824" s="30" t="s">
         <v>950</v>
       </c>
       <c r="C824" s="20" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="D824" s="22" t="s">
         <v>1650</v>
@@ -28196,21 +28196,21 @@
         <v>15</v>
       </c>
       <c r="H824" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I824" s="31" t="s">
-        <v>1593</v>
+        <v>17</v>
+      </c>
+      <c r="I824" s="20" t="s">
+        <v>1956</v>
       </c>
     </row>
     <row r="825" spans="1:9" ht="60">
       <c r="A825" s="22" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="B825" s="30" t="s">
         <v>950</v>
       </c>
       <c r="C825" s="20" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="D825" s="29"/>
       <c r="E825" s="29" t="s">
@@ -28235,7 +28235,7 @@
         <v>950</v>
       </c>
       <c r="C826" s="20" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="D826" s="22" t="s">
         <v>1562</v>
@@ -28258,13 +28258,13 @@
     </row>
     <row r="827" spans="1:9" ht="75">
       <c r="A827" s="22" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="B827" s="30" t="s">
         <v>950</v>
       </c>
       <c r="C827" s="20" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="D827" s="29" t="s">
         <v>1562</v>
@@ -28287,13 +28287,13 @@
     </row>
     <row r="828" spans="1:9" ht="75">
       <c r="A828" s="22" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="B828" s="30" t="s">
         <v>950</v>
       </c>
       <c r="C828" s="20" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="D828" s="29" t="s">
         <v>1563</v>
@@ -28316,13 +28316,13 @@
     </row>
     <row r="829" spans="1:9" ht="75">
       <c r="A829" s="22" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
       <c r="B829" s="30" t="s">
         <v>950</v>
       </c>
       <c r="C829" s="20" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="D829" s="29" t="s">
         <v>1563</v>
@@ -28349,7 +28349,7 @@
         <v>950</v>
       </c>
       <c r="C830" s="20" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="D830" s="29" t="s">
         <v>1564</v>
@@ -28378,7 +28378,7 @@
         <v>950</v>
       </c>
       <c r="C831" s="20" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="D831" s="29" t="s">
         <v>1564</v>
@@ -28401,13 +28401,13 @@
     </row>
     <row r="832" spans="1:9" ht="60">
       <c r="A832" s="22" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="B832" s="30" t="s">
         <v>950</v>
       </c>
       <c r="C832" s="20" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="D832" s="29"/>
       <c r="E832" s="29" t="s">
@@ -28426,13 +28426,13 @@
     </row>
     <row r="833" spans="1:9" ht="60">
       <c r="A833" s="22" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="B833" s="30" t="s">
         <v>950</v>
       </c>
       <c r="C833" s="20" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="D833" s="29" t="s">
         <v>1565</v>
@@ -28482,13 +28482,13 @@
     </row>
     <row r="835" spans="1:9" ht="60">
       <c r="A835" s="22" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="B835" s="30" t="s">
         <v>950</v>
       </c>
       <c r="C835" s="20" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="D835" s="29"/>
       <c r="E835" s="29" t="s">
@@ -28600,7 +28600,7 @@
         <v>950</v>
       </c>
       <c r="C839" s="20" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="D839" s="29" t="s">
         <v>1552</v>
@@ -28710,13 +28710,13 @@
     </row>
     <row r="843" spans="1:9" ht="45">
       <c r="A843" s="22" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B843" s="24" t="s">
         <v>1687</v>
       </c>
-      <c r="B843" s="24" t="s">
+      <c r="C843" s="20" t="s">
         <v>1688</v>
-      </c>
-      <c r="C843" s="20" t="s">
-        <v>1689</v>
       </c>
       <c r="D843" s="22"/>
       <c r="E843" s="29" t="s">
@@ -29045,11 +29045,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -29057,6 +29052,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:I855">

</xml_diff>

<commit_message>
[MS-OXCTABL] Update rs according to the fixed bugs.
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCTABL/MS-OXCTABL_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCTABL/MS-OXCTABL_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17030"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="120" windowWidth="15405" windowHeight="6840" tabRatio="570"/>
@@ -6147,14 +6147,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="165" formatCode="0.0.0"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="177" formatCode="0.0.0"/>
   </numFmts>
   <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -6356,13 +6356,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -6395,7 +6395,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6427,21 +6427,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -6465,6 +6450,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7357,15 +7357,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="12.375" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="3" customWidth="1"/>
     <col min="8" max="8" width="23" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.75" style="3" customWidth="1"/>
     <col min="10" max="10" width="9" style="3" customWidth="1"/>
     <col min="11" max="16384" width="9" style="3"/>
   </cols>
@@ -7407,127 +7407,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -7540,12 +7540,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -7558,12 +7558,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -7576,12 +7576,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -7594,60 +7594,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="45"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -7706,7 +7706,7 @@
       </c>
       <c r="I20" s="24"/>
     </row>
-    <row r="21" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="21" spans="1:12" s="23" customFormat="1">
       <c r="A21" s="22" t="s">
         <v>44</v>
       </c>
@@ -7731,7 +7731,7 @@
       </c>
       <c r="I21" s="24"/>
     </row>
-    <row r="22" spans="1:12" s="23" customFormat="1" ht="60">
+    <row r="22" spans="1:12" s="23" customFormat="1" ht="45">
       <c r="A22" s="22" t="s">
         <v>45</v>
       </c>
@@ -7881,7 +7881,7 @@
       </c>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="1:12" s="23" customFormat="1" ht="45">
+    <row r="28" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A28" s="22" t="s">
         <v>51</v>
       </c>
@@ -7956,7 +7956,7 @@
       </c>
       <c r="I30" s="24"/>
     </row>
-    <row r="31" spans="1:12" s="23" customFormat="1" ht="45">
+    <row r="31" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A31" s="22" t="s">
         <v>54</v>
       </c>
@@ -8231,7 +8231,7 @@
       </c>
       <c r="I41" s="31"/>
     </row>
-    <row r="42" spans="1:9" ht="30">
+    <row r="42" spans="1:9">
       <c r="A42" s="29" t="s">
         <v>65</v>
       </c>
@@ -8331,7 +8331,7 @@
       </c>
       <c r="I45" s="31"/>
     </row>
-    <row r="46" spans="1:9" ht="30">
+    <row r="46" spans="1:9">
       <c r="A46" s="29" t="s">
         <v>69</v>
       </c>
@@ -8356,7 +8356,7 @@
       </c>
       <c r="I46" s="31"/>
     </row>
-    <row r="47" spans="1:9" ht="30">
+    <row r="47" spans="1:9">
       <c r="A47" s="29" t="s">
         <v>70</v>
       </c>
@@ -8406,7 +8406,7 @@
       </c>
       <c r="I48" s="31"/>
     </row>
-    <row r="49" spans="1:9" ht="30">
+    <row r="49" spans="1:9">
       <c r="A49" s="29" t="s">
         <v>72</v>
       </c>
@@ -8481,7 +8481,7 @@
       </c>
       <c r="I51" s="31"/>
     </row>
-    <row r="52" spans="1:9" ht="60">
+    <row r="52" spans="1:9" ht="45">
       <c r="A52" s="29" t="s">
         <v>75</v>
       </c>
@@ -8606,7 +8606,7 @@
       </c>
       <c r="I56" s="31"/>
     </row>
-    <row r="57" spans="1:9" ht="45">
+    <row r="57" spans="1:9" ht="30">
       <c r="A57" s="29" t="s">
         <v>80</v>
       </c>
@@ -8631,7 +8631,7 @@
       </c>
       <c r="I57" s="31"/>
     </row>
-    <row r="58" spans="1:9" ht="60">
+    <row r="58" spans="1:9" ht="45">
       <c r="A58" s="29" t="s">
         <v>81</v>
       </c>
@@ -8658,7 +8658,7 @@
         <v>1595</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="75">
+    <row r="59" spans="1:9" ht="60">
       <c r="A59" s="29" t="s">
         <v>82</v>
       </c>
@@ -8708,7 +8708,7 @@
       </c>
       <c r="I60" s="31"/>
     </row>
-    <row r="61" spans="1:9" ht="45">
+    <row r="61" spans="1:9" ht="30">
       <c r="A61" s="29" t="s">
         <v>84</v>
       </c>
@@ -8760,7 +8760,7 @@
       </c>
       <c r="I62" s="31"/>
     </row>
-    <row r="63" spans="1:9" ht="45">
+    <row r="63" spans="1:9" ht="30">
       <c r="A63" s="29" t="s">
         <v>86</v>
       </c>
@@ -8812,7 +8812,7 @@
       </c>
       <c r="I64" s="31"/>
     </row>
-    <row r="65" spans="1:9" ht="45">
+    <row r="65" spans="1:9" ht="30">
       <c r="A65" s="29" t="s">
         <v>88</v>
       </c>
@@ -8864,7 +8864,7 @@
       </c>
       <c r="I66" s="31"/>
     </row>
-    <row r="67" spans="1:9" ht="60">
+    <row r="67" spans="1:9" ht="45">
       <c r="A67" s="29" t="s">
         <v>90</v>
       </c>
@@ -8891,7 +8891,7 @@
         <v>1596</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="45">
+    <row r="68" spans="1:9" ht="30">
       <c r="A68" s="29" t="s">
         <v>91</v>
       </c>
@@ -8918,7 +8918,7 @@
         <v>1569</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="30">
+    <row r="69" spans="1:9">
       <c r="A69" s="29" t="s">
         <v>92</v>
       </c>
@@ -8943,7 +8943,7 @@
       </c>
       <c r="I69" s="31"/>
     </row>
-    <row r="70" spans="1:9" ht="45">
+    <row r="70" spans="1:9" ht="30">
       <c r="A70" s="29" t="s">
         <v>93</v>
       </c>
@@ -8997,7 +8997,7 @@
       </c>
       <c r="I71" s="31"/>
     </row>
-    <row r="72" spans="1:9" ht="30">
+    <row r="72" spans="1:9">
       <c r="A72" s="29" t="s">
         <v>95</v>
       </c>
@@ -9174,7 +9174,7 @@
       </c>
       <c r="I78" s="31"/>
     </row>
-    <row r="79" spans="1:9" ht="30">
+    <row r="79" spans="1:9">
       <c r="A79" s="29" t="s">
         <v>102</v>
       </c>
@@ -9351,7 +9351,7 @@
       </c>
       <c r="I85" s="31"/>
     </row>
-    <row r="86" spans="1:9" ht="60">
+    <row r="86" spans="1:9" ht="45">
       <c r="A86" s="29" t="s">
         <v>109</v>
       </c>
@@ -9628,7 +9628,7 @@
       </c>
       <c r="I96" s="31"/>
     </row>
-    <row r="97" spans="1:9" ht="30">
+    <row r="97" spans="1:9">
       <c r="A97" s="29" t="s">
         <v>120</v>
       </c>
@@ -9653,7 +9653,7 @@
       </c>
       <c r="I97" s="31"/>
     </row>
-    <row r="98" spans="1:9" ht="45">
+    <row r="98" spans="1:9" ht="30">
       <c r="A98" s="29" t="s">
         <v>121</v>
       </c>
@@ -9803,7 +9803,7 @@
       </c>
       <c r="I103" s="31"/>
     </row>
-    <row r="104" spans="1:9" ht="30">
+    <row r="104" spans="1:9">
       <c r="A104" s="29" t="s">
         <v>127</v>
       </c>
@@ -9853,7 +9853,7 @@
       </c>
       <c r="I105" s="31"/>
     </row>
-    <row r="106" spans="1:9" ht="45">
+    <row r="106" spans="1:9" ht="30">
       <c r="A106" s="29" t="s">
         <v>129</v>
       </c>
@@ -9928,7 +9928,7 @@
       </c>
       <c r="I108" s="31"/>
     </row>
-    <row r="109" spans="1:9" ht="60">
+    <row r="109" spans="1:9" ht="45">
       <c r="A109" s="29" t="s">
         <v>132</v>
       </c>
@@ -9978,7 +9978,7 @@
       </c>
       <c r="I110" s="31"/>
     </row>
-    <row r="111" spans="1:9" ht="60">
+    <row r="111" spans="1:9" ht="45">
       <c r="A111" s="29" t="s">
         <v>134</v>
       </c>
@@ -10053,7 +10053,7 @@
       </c>
       <c r="I113" s="31"/>
     </row>
-    <row r="114" spans="1:9" ht="60">
+    <row r="114" spans="1:9" ht="45">
       <c r="A114" s="29" t="s">
         <v>137</v>
       </c>
@@ -10103,7 +10103,7 @@
       </c>
       <c r="I115" s="31"/>
     </row>
-    <row r="116" spans="1:9" ht="45">
+    <row r="116" spans="1:9" ht="30">
       <c r="A116" s="29" t="s">
         <v>139</v>
       </c>
@@ -10128,7 +10128,7 @@
       </c>
       <c r="I116" s="31"/>
     </row>
-    <row r="117" spans="1:9" ht="45">
+    <row r="117" spans="1:9" ht="30">
       <c r="A117" s="29" t="s">
         <v>140</v>
       </c>
@@ -10178,7 +10178,7 @@
       </c>
       <c r="I118" s="31"/>
     </row>
-    <row r="119" spans="1:9" ht="60">
+    <row r="119" spans="1:9" ht="45">
       <c r="A119" s="29" t="s">
         <v>142</v>
       </c>
@@ -10278,7 +10278,7 @@
       </c>
       <c r="I122" s="31"/>
     </row>
-    <row r="123" spans="1:9" ht="45">
+    <row r="123" spans="1:9" ht="30">
       <c r="A123" s="29" t="s">
         <v>146</v>
       </c>
@@ -10630,7 +10630,7 @@
       </c>
       <c r="I136" s="31"/>
     </row>
-    <row r="137" spans="1:9" ht="30">
+    <row r="137" spans="1:9">
       <c r="A137" s="29" t="s">
         <v>160</v>
       </c>
@@ -10655,7 +10655,7 @@
       </c>
       <c r="I137" s="31"/>
     </row>
-    <row r="138" spans="1:9" ht="30">
+    <row r="138" spans="1:9">
       <c r="A138" s="29" t="s">
         <v>161</v>
       </c>
@@ -11007,7 +11007,7 @@
       </c>
       <c r="I151" s="31"/>
     </row>
-    <row r="152" spans="1:9" ht="60">
+    <row r="152" spans="1:9" ht="45">
       <c r="A152" s="29" t="s">
         <v>175</v>
       </c>
@@ -11032,7 +11032,7 @@
       </c>
       <c r="I152" s="31"/>
     </row>
-    <row r="153" spans="1:9" ht="60">
+    <row r="153" spans="1:9" ht="45">
       <c r="A153" s="29" t="s">
         <v>176</v>
       </c>
@@ -11057,7 +11057,7 @@
       </c>
       <c r="I153" s="31"/>
     </row>
-    <row r="154" spans="1:9" ht="30">
+    <row r="154" spans="1:9">
       <c r="A154" s="29" t="s">
         <v>177</v>
       </c>
@@ -11082,7 +11082,7 @@
       </c>
       <c r="I154" s="31"/>
     </row>
-    <row r="155" spans="1:9" ht="45">
+    <row r="155" spans="1:9" ht="30">
       <c r="A155" s="29" t="s">
         <v>178</v>
       </c>
@@ -11157,7 +11157,7 @@
       </c>
       <c r="I157" s="31"/>
     </row>
-    <row r="158" spans="1:9" ht="30">
+    <row r="158" spans="1:9">
       <c r="A158" s="29" t="s">
         <v>181</v>
       </c>
@@ -11182,7 +11182,7 @@
       </c>
       <c r="I158" s="31"/>
     </row>
-    <row r="159" spans="1:9" ht="30">
+    <row r="159" spans="1:9">
       <c r="A159" s="29" t="s">
         <v>182</v>
       </c>
@@ -11207,7 +11207,7 @@
       </c>
       <c r="I159" s="31"/>
     </row>
-    <row r="160" spans="1:9" ht="30">
+    <row r="160" spans="1:9">
       <c r="A160" s="29" t="s">
         <v>183</v>
       </c>
@@ -11232,7 +11232,7 @@
       </c>
       <c r="I160" s="31"/>
     </row>
-    <row r="161" spans="1:9" ht="30">
+    <row r="161" spans="1:9">
       <c r="A161" s="29" t="s">
         <v>184</v>
       </c>
@@ -11309,7 +11309,7 @@
       </c>
       <c r="I163" s="31"/>
     </row>
-    <row r="164" spans="1:9" ht="30">
+    <row r="164" spans="1:9">
       <c r="A164" s="29" t="s">
         <v>187</v>
       </c>
@@ -11384,7 +11384,7 @@
       </c>
       <c r="I166" s="31"/>
     </row>
-    <row r="167" spans="1:9" ht="45">
+    <row r="167" spans="1:9" ht="30">
       <c r="A167" s="29" t="s">
         <v>190</v>
       </c>
@@ -11484,7 +11484,7 @@
       </c>
       <c r="I170" s="31"/>
     </row>
-    <row r="171" spans="1:9" ht="45">
+    <row r="171" spans="1:9" ht="30">
       <c r="A171" s="29" t="s">
         <v>194</v>
       </c>
@@ -11509,7 +11509,7 @@
       </c>
       <c r="I171" s="31"/>
     </row>
-    <row r="172" spans="1:9" ht="45">
+    <row r="172" spans="1:9" ht="30">
       <c r="A172" s="29" t="s">
         <v>195</v>
       </c>
@@ -11559,7 +11559,7 @@
       </c>
       <c r="I173" s="31"/>
     </row>
-    <row r="174" spans="1:9" ht="45">
+    <row r="174" spans="1:9" ht="30">
       <c r="A174" s="29" t="s">
         <v>197</v>
       </c>
@@ -11834,7 +11834,7 @@
       </c>
       <c r="I184" s="31"/>
     </row>
-    <row r="185" spans="1:9" ht="45">
+    <row r="185" spans="1:9" ht="30">
       <c r="A185" s="29" t="s">
         <v>208</v>
       </c>
@@ -11886,7 +11886,7 @@
       </c>
       <c r="I186" s="31"/>
     </row>
-    <row r="187" spans="1:9" ht="45">
+    <row r="187" spans="1:9" ht="30">
       <c r="A187" s="29" t="s">
         <v>210</v>
       </c>
@@ -12063,7 +12063,7 @@
       </c>
       <c r="I193" s="31"/>
     </row>
-    <row r="194" spans="1:9" ht="45">
+    <row r="194" spans="1:9" ht="30">
       <c r="A194" s="29" t="s">
         <v>217</v>
       </c>
@@ -12444,7 +12444,7 @@
         <v>1603</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="45">
+    <row r="209" spans="1:9" ht="30">
       <c r="A209" s="29" t="s">
         <v>232</v>
       </c>
@@ -12669,7 +12669,7 @@
       </c>
       <c r="I217" s="31"/>
     </row>
-    <row r="218" spans="1:9" ht="30">
+    <row r="218" spans="1:9">
       <c r="A218" s="29" t="s">
         <v>241</v>
       </c>
@@ -12871,7 +12871,7 @@
       </c>
       <c r="I225" s="31"/>
     </row>
-    <row r="226" spans="1:9" ht="45">
+    <row r="226" spans="1:9" ht="30">
       <c r="A226" s="29" t="s">
         <v>249</v>
       </c>
@@ -12896,7 +12896,7 @@
       </c>
       <c r="I226" s="31"/>
     </row>
-    <row r="227" spans="1:9" ht="45">
+    <row r="227" spans="1:9" ht="30">
       <c r="A227" s="29" t="s">
         <v>250</v>
       </c>
@@ -12921,7 +12921,7 @@
       </c>
       <c r="I227" s="31"/>
     </row>
-    <row r="228" spans="1:9" ht="30">
+    <row r="228" spans="1:9">
       <c r="A228" s="29" t="s">
         <v>251</v>
       </c>
@@ -13071,7 +13071,7 @@
       </c>
       <c r="I233" s="31"/>
     </row>
-    <row r="234" spans="1:9" ht="30">
+    <row r="234" spans="1:9">
       <c r="A234" s="29" t="s">
         <v>257</v>
       </c>
@@ -13173,7 +13173,7 @@
         <v>1605</v>
       </c>
     </row>
-    <row r="238" spans="1:9" ht="45">
+    <row r="238" spans="1:9" ht="30">
       <c r="A238" s="29" t="s">
         <v>261</v>
       </c>
@@ -13198,7 +13198,7 @@
       </c>
       <c r="I238" s="31"/>
     </row>
-    <row r="239" spans="1:9" ht="60">
+    <row r="239" spans="1:9" ht="45">
       <c r="A239" s="29" t="s">
         <v>262</v>
       </c>
@@ -13373,7 +13373,7 @@
       </c>
       <c r="I245" s="31"/>
     </row>
-    <row r="246" spans="1:9" ht="45">
+    <row r="246" spans="1:9" ht="30">
       <c r="A246" s="29" t="s">
         <v>269</v>
       </c>
@@ -13473,7 +13473,7 @@
       </c>
       <c r="I249" s="31"/>
     </row>
-    <row r="250" spans="1:9" ht="30">
+    <row r="250" spans="1:9">
       <c r="A250" s="29" t="s">
         <v>273</v>
       </c>
@@ -13671,11 +13671,11 @@
         <v>15</v>
       </c>
       <c r="H257" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I257" s="31"/>
     </row>
-    <row r="258" spans="1:9" ht="45">
+    <row r="258" spans="1:9" ht="30">
       <c r="A258" s="29" t="s">
         <v>281</v>
       </c>
@@ -13721,11 +13721,11 @@
         <v>15</v>
       </c>
       <c r="H259" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I259" s="31"/>
     </row>
-    <row r="260" spans="1:9" ht="45">
+    <row r="260" spans="1:9" ht="30">
       <c r="A260" s="29" t="s">
         <v>283</v>
       </c>
@@ -13775,7 +13775,7 @@
       </c>
       <c r="I261" s="31"/>
     </row>
-    <row r="262" spans="1:9" ht="45">
+    <row r="262" spans="1:9" ht="30">
       <c r="A262" s="29" t="s">
         <v>285</v>
       </c>
@@ -13800,7 +13800,7 @@
       </c>
       <c r="I262" s="31"/>
     </row>
-    <row r="263" spans="1:9" ht="45">
+    <row r="263" spans="1:9" ht="30">
       <c r="A263" s="29" t="s">
         <v>286</v>
       </c>
@@ -13825,7 +13825,7 @@
       </c>
       <c r="I263" s="31"/>
     </row>
-    <row r="264" spans="1:9" ht="30">
+    <row r="264" spans="1:9">
       <c r="A264" s="29" t="s">
         <v>287</v>
       </c>
@@ -14202,7 +14202,7 @@
         <v>1607</v>
       </c>
     </row>
-    <row r="279" spans="1:9" ht="45">
+    <row r="279" spans="1:9" ht="30">
       <c r="A279" s="29" t="s">
         <v>302</v>
       </c>
@@ -14279,7 +14279,7 @@
       </c>
       <c r="I281" s="31"/>
     </row>
-    <row r="282" spans="1:9" ht="45">
+    <row r="282" spans="1:9" ht="30">
       <c r="A282" s="29" t="s">
         <v>305</v>
       </c>
@@ -14656,7 +14656,7 @@
       </c>
       <c r="I296" s="31"/>
     </row>
-    <row r="297" spans="1:9" ht="45">
+    <row r="297" spans="1:9" ht="30">
       <c r="A297" s="29" t="s">
         <v>320</v>
       </c>
@@ -15083,7 +15083,7 @@
       </c>
       <c r="I313" s="31"/>
     </row>
-    <row r="314" spans="1:9" ht="30">
+    <row r="314" spans="1:9">
       <c r="A314" s="29" t="s">
         <v>337</v>
       </c>
@@ -15108,7 +15108,7 @@
       </c>
       <c r="I314" s="31"/>
     </row>
-    <row r="315" spans="1:9" ht="30">
+    <row r="315" spans="1:9">
       <c r="A315" s="29" t="s">
         <v>338</v>
       </c>
@@ -15133,7 +15133,7 @@
       </c>
       <c r="I315" s="31"/>
     </row>
-    <row r="316" spans="1:9" ht="30">
+    <row r="316" spans="1:9">
       <c r="A316" s="29" t="s">
         <v>339</v>
       </c>
@@ -15208,7 +15208,7 @@
       </c>
       <c r="I318" s="31"/>
     </row>
-    <row r="319" spans="1:9" ht="30">
+    <row r="319" spans="1:9">
       <c r="A319" s="29" t="s">
         <v>342</v>
       </c>
@@ -15310,7 +15310,7 @@
         <v>1881</v>
       </c>
     </row>
-    <row r="323" spans="1:9" ht="45">
+    <row r="323" spans="1:9" ht="30">
       <c r="A323" s="29" t="s">
         <v>346</v>
       </c>
@@ -15356,11 +15356,11 @@
         <v>15</v>
       </c>
       <c r="H324" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I324" s="31"/>
     </row>
-    <row r="325" spans="1:9" ht="45">
+    <row r="325" spans="1:9" ht="30">
       <c r="A325" s="29" t="s">
         <v>348</v>
       </c>
@@ -15410,7 +15410,7 @@
       </c>
       <c r="I326" s="31"/>
     </row>
-    <row r="327" spans="1:9" ht="45">
+    <row r="327" spans="1:9" ht="30">
       <c r="A327" s="29" t="s">
         <v>350</v>
       </c>
@@ -15562,7 +15562,7 @@
       </c>
       <c r="I332" s="35"/>
     </row>
-    <row r="333" spans="1:9" ht="45">
+    <row r="333" spans="1:9" ht="30">
       <c r="A333" s="22" t="s">
         <v>355</v>
       </c>
@@ -15587,7 +15587,7 @@
       </c>
       <c r="I333" s="31"/>
     </row>
-    <row r="334" spans="1:9" ht="45">
+    <row r="334" spans="1:9" ht="30">
       <c r="A334" s="29" t="s">
         <v>356</v>
       </c>
@@ -15941,7 +15941,7 @@
       </c>
       <c r="I347" s="31"/>
     </row>
-    <row r="348" spans="1:9" ht="60">
+    <row r="348" spans="1:9" ht="45">
       <c r="A348" s="29" t="s">
         <v>370</v>
       </c>
@@ -16016,7 +16016,7 @@
       </c>
       <c r="I350" s="31"/>
     </row>
-    <row r="351" spans="1:9" ht="45">
+    <row r="351" spans="1:9" ht="30">
       <c r="A351" s="29" t="s">
         <v>373</v>
       </c>
@@ -16191,7 +16191,7 @@
       </c>
       <c r="I357" s="31"/>
     </row>
-    <row r="358" spans="1:9" ht="45">
+    <row r="358" spans="1:9" ht="30">
       <c r="A358" s="29" t="s">
         <v>380</v>
       </c>
@@ -16370,7 +16370,7 @@
         <v>1615</v>
       </c>
     </row>
-    <row r="365" spans="1:9" ht="30">
+    <row r="365" spans="1:9">
       <c r="A365" s="29" t="s">
         <v>387</v>
       </c>
@@ -16545,7 +16545,7 @@
       </c>
       <c r="I371" s="31"/>
     </row>
-    <row r="372" spans="1:9" ht="45">
+    <row r="372" spans="1:9" ht="30">
       <c r="A372" s="29" t="s">
         <v>394</v>
       </c>
@@ -16797,7 +16797,7 @@
       </c>
       <c r="I381" s="31"/>
     </row>
-    <row r="382" spans="1:9" ht="45">
+    <row r="382" spans="1:9" ht="30">
       <c r="A382" s="29" t="s">
         <v>404</v>
       </c>
@@ -16999,7 +16999,7 @@
       </c>
       <c r="I389" s="31"/>
     </row>
-    <row r="390" spans="1:9" ht="60">
+    <row r="390" spans="1:9" ht="45">
       <c r="A390" s="29" t="s">
         <v>412</v>
       </c>
@@ -17199,7 +17199,7 @@
       </c>
       <c r="I397" s="31"/>
     </row>
-    <row r="398" spans="1:9" ht="30">
+    <row r="398" spans="1:9">
       <c r="A398" s="29" t="s">
         <v>420</v>
       </c>
@@ -17224,7 +17224,7 @@
       </c>
       <c r="I398" s="31"/>
     </row>
-    <row r="399" spans="1:9" ht="45">
+    <row r="399" spans="1:9" ht="30">
       <c r="A399" s="29" t="s">
         <v>421</v>
       </c>
@@ -17474,7 +17474,7 @@
       </c>
       <c r="I408" s="31"/>
     </row>
-    <row r="409" spans="1:9" ht="60">
+    <row r="409" spans="1:9" ht="45">
       <c r="A409" s="29" t="s">
         <v>431</v>
       </c>
@@ -17524,7 +17524,7 @@
       </c>
       <c r="I410" s="31"/>
     </row>
-    <row r="411" spans="1:9" ht="30">
+    <row r="411" spans="1:9">
       <c r="A411" s="29" t="s">
         <v>433</v>
       </c>
@@ -17624,7 +17624,7 @@
       </c>
       <c r="I414" s="31"/>
     </row>
-    <row r="415" spans="1:9" ht="45">
+    <row r="415" spans="1:9" ht="30">
       <c r="A415" s="29" t="s">
         <v>437</v>
       </c>
@@ -17649,7 +17649,7 @@
       </c>
       <c r="I415" s="31"/>
     </row>
-    <row r="416" spans="1:9" ht="45">
+    <row r="416" spans="1:9" ht="30">
       <c r="A416" s="29" t="s">
         <v>438</v>
       </c>
@@ -17674,7 +17674,7 @@
       </c>
       <c r="I416" s="31"/>
     </row>
-    <row r="417" spans="1:9" ht="45">
+    <row r="417" spans="1:9" ht="30">
       <c r="A417" s="29" t="s">
         <v>439</v>
       </c>
@@ -17699,7 +17699,7 @@
       </c>
       <c r="I417" s="31"/>
     </row>
-    <row r="418" spans="1:9" ht="30">
+    <row r="418" spans="1:9">
       <c r="A418" s="29" t="s">
         <v>440</v>
       </c>
@@ -17974,7 +17974,7 @@
       </c>
       <c r="I428" s="31"/>
     </row>
-    <row r="429" spans="1:9" ht="45">
+    <row r="429" spans="1:9" ht="30">
       <c r="A429" s="29" t="s">
         <v>451</v>
       </c>
@@ -17999,7 +17999,7 @@
       </c>
       <c r="I429" s="31"/>
     </row>
-    <row r="430" spans="1:9" ht="45">
+    <row r="430" spans="1:9" ht="30">
       <c r="A430" s="29" t="s">
         <v>452</v>
       </c>
@@ -18099,7 +18099,7 @@
       </c>
       <c r="I433" s="31"/>
     </row>
-    <row r="434" spans="1:9" ht="75">
+    <row r="434" spans="1:9" ht="60">
       <c r="A434" s="29" t="s">
         <v>456</v>
       </c>
@@ -18224,7 +18224,7 @@
       </c>
       <c r="I438" s="31"/>
     </row>
-    <row r="439" spans="1:9" ht="45">
+    <row r="439" spans="1:9" ht="30">
       <c r="A439" s="29" t="s">
         <v>461</v>
       </c>
@@ -18249,7 +18249,7 @@
       </c>
       <c r="I439" s="31"/>
     </row>
-    <row r="440" spans="1:9" ht="45">
+    <row r="440" spans="1:9" ht="30">
       <c r="A440" s="29" t="s">
         <v>462</v>
       </c>
@@ -18349,7 +18349,7 @@
       </c>
       <c r="I443" s="31"/>
     </row>
-    <row r="444" spans="1:9" ht="60">
+    <row r="444" spans="1:9" ht="45">
       <c r="A444" s="29" t="s">
         <v>466</v>
       </c>
@@ -18399,7 +18399,7 @@
       </c>
       <c r="I445" s="31"/>
     </row>
-    <row r="446" spans="1:9" ht="45">
+    <row r="446" spans="1:9" ht="30">
       <c r="A446" s="29" t="s">
         <v>468</v>
       </c>
@@ -18449,7 +18449,7 @@
       </c>
       <c r="I447" s="31"/>
     </row>
-    <row r="448" spans="1:9" ht="45">
+    <row r="448" spans="1:9" ht="30">
       <c r="A448" s="29" t="s">
         <v>470</v>
       </c>
@@ -18499,7 +18499,7 @@
       </c>
       <c r="I449" s="31"/>
     </row>
-    <row r="450" spans="1:9" ht="45">
+    <row r="450" spans="1:9" ht="30">
       <c r="A450" s="29" t="s">
         <v>472</v>
       </c>
@@ -18524,7 +18524,7 @@
       </c>
       <c r="I450" s="31"/>
     </row>
-    <row r="451" spans="1:9" ht="45">
+    <row r="451" spans="1:9" ht="30">
       <c r="A451" s="29" t="s">
         <v>473</v>
       </c>
@@ -18649,7 +18649,7 @@
       </c>
       <c r="I455" s="31"/>
     </row>
-    <row r="456" spans="1:9" ht="45">
+    <row r="456" spans="1:9" ht="30">
       <c r="A456" s="29" t="s">
         <v>478</v>
       </c>
@@ -18699,7 +18699,7 @@
       </c>
       <c r="I457" s="31"/>
     </row>
-    <row r="458" spans="1:9" ht="75">
+    <row r="458" spans="1:9" ht="60">
       <c r="A458" s="29" t="s">
         <v>480</v>
       </c>
@@ -18724,7 +18724,7 @@
       </c>
       <c r="I458" s="31"/>
     </row>
-    <row r="459" spans="1:9" ht="45">
+    <row r="459" spans="1:9" ht="30">
       <c r="A459" s="29" t="s">
         <v>481</v>
       </c>
@@ -18749,7 +18749,7 @@
       </c>
       <c r="I459" s="31"/>
     </row>
-    <row r="460" spans="1:9" ht="75">
+    <row r="460" spans="1:9" ht="60">
       <c r="A460" s="29" t="s">
         <v>482</v>
       </c>
@@ -18849,7 +18849,7 @@
       </c>
       <c r="I463" s="31"/>
     </row>
-    <row r="464" spans="1:9" ht="45">
+    <row r="464" spans="1:9" ht="30">
       <c r="A464" s="29" t="s">
         <v>486</v>
       </c>
@@ -18974,7 +18974,7 @@
       </c>
       <c r="I468" s="31"/>
     </row>
-    <row r="469" spans="1:9" ht="45">
+    <row r="469" spans="1:9" ht="30">
       <c r="A469" s="29" t="s">
         <v>491</v>
       </c>
@@ -18999,7 +18999,7 @@
       </c>
       <c r="I469" s="31"/>
     </row>
-    <row r="470" spans="1:9" ht="60">
+    <row r="470" spans="1:9" ht="45">
       <c r="A470" s="29" t="s">
         <v>492</v>
       </c>
@@ -19024,7 +19024,7 @@
       </c>
       <c r="I470" s="31"/>
     </row>
-    <row r="471" spans="1:9" ht="60">
+    <row r="471" spans="1:9" ht="45">
       <c r="A471" s="29" t="s">
         <v>493</v>
       </c>
@@ -19049,7 +19049,7 @@
       </c>
       <c r="I471" s="31"/>
     </row>
-    <row r="472" spans="1:9" ht="45">
+    <row r="472" spans="1:9" ht="30">
       <c r="A472" s="29" t="s">
         <v>494</v>
       </c>
@@ -19099,7 +19099,7 @@
       </c>
       <c r="I473" s="31"/>
     </row>
-    <row r="474" spans="1:9" ht="45">
+    <row r="474" spans="1:9" ht="30">
       <c r="A474" s="29" t="s">
         <v>496</v>
       </c>
@@ -19174,7 +19174,7 @@
       </c>
       <c r="I476" s="31"/>
     </row>
-    <row r="477" spans="1:9" ht="45">
+    <row r="477" spans="1:9" ht="30">
       <c r="A477" s="29" t="s">
         <v>499</v>
       </c>
@@ -19274,7 +19274,7 @@
       </c>
       <c r="I480" s="31"/>
     </row>
-    <row r="481" spans="1:9" ht="45">
+    <row r="481" spans="1:9" ht="30">
       <c r="A481" s="29" t="s">
         <v>503</v>
       </c>
@@ -19299,7 +19299,7 @@
       </c>
       <c r="I481" s="31"/>
     </row>
-    <row r="482" spans="1:9" ht="60">
+    <row r="482" spans="1:9" ht="45">
       <c r="A482" s="29" t="s">
         <v>504</v>
       </c>
@@ -19324,7 +19324,7 @@
       </c>
       <c r="I482" s="31"/>
     </row>
-    <row r="483" spans="1:9" ht="45">
+    <row r="483" spans="1:9" ht="30">
       <c r="A483" s="29" t="s">
         <v>505</v>
       </c>
@@ -19399,7 +19399,7 @@
       </c>
       <c r="I485" s="31"/>
     </row>
-    <row r="486" spans="1:9" ht="60">
+    <row r="486" spans="1:9" ht="45">
       <c r="A486" s="29" t="s">
         <v>508</v>
       </c>
@@ -19424,7 +19424,7 @@
       </c>
       <c r="I486" s="31"/>
     </row>
-    <row r="487" spans="1:9" ht="60">
+    <row r="487" spans="1:9" ht="45">
       <c r="A487" s="29" t="s">
         <v>509</v>
       </c>
@@ -19449,7 +19449,7 @@
       </c>
       <c r="I487" s="31"/>
     </row>
-    <row r="488" spans="1:9" ht="60">
+    <row r="488" spans="1:9" ht="45">
       <c r="A488" s="29" t="s">
         <v>510</v>
       </c>
@@ -19576,7 +19576,7 @@
       </c>
       <c r="I492" s="31"/>
     </row>
-    <row r="493" spans="1:9" ht="45">
+    <row r="493" spans="1:9" ht="30">
       <c r="A493" s="29" t="s">
         <v>515</v>
       </c>
@@ -19676,7 +19676,7 @@
       </c>
       <c r="I496" s="31"/>
     </row>
-    <row r="497" spans="1:9" ht="45">
+    <row r="497" spans="1:9" ht="30">
       <c r="A497" s="29" t="s">
         <v>519</v>
       </c>
@@ -19776,7 +19776,7 @@
       </c>
       <c r="I500" s="31"/>
     </row>
-    <row r="501" spans="1:9" ht="60">
+    <row r="501" spans="1:9" ht="45">
       <c r="A501" s="29" t="s">
         <v>523</v>
       </c>
@@ -19803,7 +19803,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="502" spans="1:9" ht="60">
+    <row r="502" spans="1:9" ht="45">
       <c r="A502" s="29" t="s">
         <v>524</v>
       </c>
@@ -19830,7 +19830,7 @@
         <v>1574</v>
       </c>
     </row>
-    <row r="503" spans="1:9" ht="60">
+    <row r="503" spans="1:9" ht="45">
       <c r="A503" s="29" t="s">
         <v>525</v>
       </c>
@@ -19857,7 +19857,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="504" spans="1:9" ht="60">
+    <row r="504" spans="1:9" ht="45">
       <c r="A504" s="29" t="s">
         <v>526</v>
       </c>
@@ -19884,7 +19884,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="505" spans="1:9" ht="60">
+    <row r="505" spans="1:9" ht="45">
       <c r="A505" s="29" t="s">
         <v>527</v>
       </c>
@@ -19934,7 +19934,7 @@
       </c>
       <c r="I506" s="31"/>
     </row>
-    <row r="507" spans="1:9" ht="45">
+    <row r="507" spans="1:9" ht="30">
       <c r="A507" s="29" t="s">
         <v>529</v>
       </c>
@@ -19984,7 +19984,7 @@
       </c>
       <c r="I508" s="31"/>
     </row>
-    <row r="509" spans="1:9" ht="60">
+    <row r="509" spans="1:9" ht="45">
       <c r="A509" s="29" t="s">
         <v>531</v>
       </c>
@@ -20009,7 +20009,7 @@
       </c>
       <c r="I509" s="31"/>
     </row>
-    <row r="510" spans="1:9" ht="60">
+    <row r="510" spans="1:9" ht="45">
       <c r="A510" s="29" t="s">
         <v>532</v>
       </c>
@@ -20034,7 +20034,7 @@
       </c>
       <c r="I510" s="31"/>
     </row>
-    <row r="511" spans="1:9" ht="60">
+    <row r="511" spans="1:9" ht="45">
       <c r="A511" s="29" t="s">
         <v>533</v>
       </c>
@@ -20084,7 +20084,7 @@
       </c>
       <c r="I512" s="31"/>
     </row>
-    <row r="513" spans="1:9" ht="45">
+    <row r="513" spans="1:9" ht="30">
       <c r="A513" s="29" t="s">
         <v>535</v>
       </c>
@@ -20109,7 +20109,7 @@
       </c>
       <c r="I513" s="31"/>
     </row>
-    <row r="514" spans="1:9" ht="45">
+    <row r="514" spans="1:9" ht="30">
       <c r="A514" s="29" t="s">
         <v>536</v>
       </c>
@@ -20159,7 +20159,7 @@
       </c>
       <c r="I515" s="31"/>
     </row>
-    <row r="516" spans="1:9" ht="45">
+    <row r="516" spans="1:9" ht="30">
       <c r="A516" s="29" t="s">
         <v>538</v>
       </c>
@@ -20186,7 +20186,7 @@
         <v>1577</v>
       </c>
     </row>
-    <row r="517" spans="1:9" ht="45">
+    <row r="517" spans="1:9" ht="30">
       <c r="A517" s="22" t="s">
         <v>539</v>
       </c>
@@ -20213,7 +20213,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="518" spans="1:9" ht="45">
+    <row r="518" spans="1:9" ht="30">
       <c r="A518" s="22" t="s">
         <v>1797</v>
       </c>
@@ -20240,7 +20240,7 @@
         <v>1941</v>
       </c>
     </row>
-    <row r="519" spans="1:9" ht="45">
+    <row r="519" spans="1:9" ht="30">
       <c r="A519" s="22" t="s">
         <v>1798</v>
       </c>
@@ -20267,7 +20267,7 @@
         <v>1942</v>
       </c>
     </row>
-    <row r="520" spans="1:9" ht="45">
+    <row r="520" spans="1:9" ht="30">
       <c r="A520" s="22" t="s">
         <v>1799</v>
       </c>
@@ -20294,7 +20294,7 @@
         <v>1943</v>
       </c>
     </row>
-    <row r="521" spans="1:9" ht="45">
+    <row r="521" spans="1:9" ht="30">
       <c r="A521" s="22" t="s">
         <v>1800</v>
       </c>
@@ -20321,7 +20321,7 @@
         <v>1944</v>
       </c>
     </row>
-    <row r="522" spans="1:9" ht="45">
+    <row r="522" spans="1:9" ht="30">
       <c r="A522" s="22" t="s">
         <v>1801</v>
       </c>
@@ -20348,7 +20348,7 @@
         <v>1945</v>
       </c>
     </row>
-    <row r="523" spans="1:9" ht="45">
+    <row r="523" spans="1:9" ht="30">
       <c r="A523" s="22" t="s">
         <v>1802</v>
       </c>
@@ -20375,7 +20375,7 @@
         <v>1946</v>
       </c>
     </row>
-    <row r="524" spans="1:9" ht="45">
+    <row r="524" spans="1:9" ht="30">
       <c r="A524" s="22" t="s">
         <v>1803</v>
       </c>
@@ -20402,7 +20402,7 @@
         <v>1947</v>
       </c>
     </row>
-    <row r="525" spans="1:9" ht="45">
+    <row r="525" spans="1:9" ht="30">
       <c r="A525" s="29" t="s">
         <v>540</v>
       </c>
@@ -20454,7 +20454,7 @@
       </c>
       <c r="I526" s="31"/>
     </row>
-    <row r="527" spans="1:9" ht="45">
+    <row r="527" spans="1:9" ht="30">
       <c r="A527" s="29" t="s">
         <v>542</v>
       </c>
@@ -20481,7 +20481,7 @@
         <v>1580</v>
       </c>
     </row>
-    <row r="528" spans="1:9" ht="30">
+    <row r="528" spans="1:9">
       <c r="A528" s="29" t="s">
         <v>543</v>
       </c>
@@ -20506,7 +20506,7 @@
       </c>
       <c r="I528" s="31"/>
     </row>
-    <row r="529" spans="1:9" ht="30">
+    <row r="529" spans="1:9">
       <c r="A529" s="29" t="s">
         <v>544</v>
       </c>
@@ -20533,7 +20533,7 @@
       </c>
       <c r="I529" s="31"/>
     </row>
-    <row r="530" spans="1:9" ht="30">
+    <row r="530" spans="1:9">
       <c r="A530" s="29" t="s">
         <v>545</v>
       </c>
@@ -20560,7 +20560,7 @@
       </c>
       <c r="I530" s="31"/>
     </row>
-    <row r="531" spans="1:9" ht="30">
+    <row r="531" spans="1:9">
       <c r="A531" s="29" t="s">
         <v>546</v>
       </c>
@@ -20637,7 +20637,7 @@
       </c>
       <c r="I533" s="31"/>
     </row>
-    <row r="534" spans="1:9" ht="30">
+    <row r="534" spans="1:9">
       <c r="A534" s="29" t="s">
         <v>549</v>
       </c>
@@ -20864,7 +20864,7 @@
       </c>
       <c r="I542" s="31"/>
     </row>
-    <row r="543" spans="1:9" ht="45">
+    <row r="543" spans="1:9" ht="30">
       <c r="A543" s="29" t="s">
         <v>558</v>
       </c>
@@ -20891,7 +20891,7 @@
         <v>1581</v>
       </c>
     </row>
-    <row r="544" spans="1:9" ht="30">
+    <row r="544" spans="1:9">
       <c r="A544" s="29" t="s">
         <v>559</v>
       </c>
@@ -20916,7 +20916,7 @@
       </c>
       <c r="I544" s="31"/>
     </row>
-    <row r="545" spans="1:9" ht="45">
+    <row r="545" spans="1:9" ht="30">
       <c r="A545" s="29" t="s">
         <v>560</v>
       </c>
@@ -20968,7 +20968,7 @@
       </c>
       <c r="I546" s="31"/>
     </row>
-    <row r="547" spans="1:9" ht="90">
+    <row r="547" spans="1:9" ht="75">
       <c r="A547" s="29" t="s">
         <v>562</v>
       </c>
@@ -20993,7 +20993,7 @@
       </c>
       <c r="I547" s="31"/>
     </row>
-    <row r="548" spans="1:9" ht="30">
+    <row r="548" spans="1:9">
       <c r="A548" s="29" t="s">
         <v>563</v>
       </c>
@@ -21018,7 +21018,7 @@
       </c>
       <c r="I548" s="31"/>
     </row>
-    <row r="549" spans="1:9" ht="30">
+    <row r="549" spans="1:9">
       <c r="A549" s="29" t="s">
         <v>564</v>
       </c>
@@ -21168,7 +21168,7 @@
       </c>
       <c r="I554" s="31"/>
     </row>
-    <row r="555" spans="1:9" ht="45">
+    <row r="555" spans="1:9" ht="30">
       <c r="A555" s="29" t="s">
         <v>570</v>
       </c>
@@ -21220,7 +21220,7 @@
       </c>
       <c r="I556" s="31"/>
     </row>
-    <row r="557" spans="1:9" ht="60">
+    <row r="557" spans="1:9" ht="45">
       <c r="A557" s="29" t="s">
         <v>572</v>
       </c>
@@ -21353,7 +21353,7 @@
       </c>
       <c r="I561" s="31"/>
     </row>
-    <row r="562" spans="1:9" ht="30">
+    <row r="562" spans="1:9">
       <c r="A562" s="29" t="s">
         <v>576</v>
       </c>
@@ -21378,7 +21378,7 @@
       </c>
       <c r="I562" s="31"/>
     </row>
-    <row r="563" spans="1:9" ht="30">
+    <row r="563" spans="1:9">
       <c r="A563" s="29" t="s">
         <v>577</v>
       </c>
@@ -21428,7 +21428,7 @@
       </c>
       <c r="I564" s="31"/>
     </row>
-    <row r="565" spans="1:9" ht="45">
+    <row r="565" spans="1:9" ht="30">
       <c r="A565" s="29" t="s">
         <v>579</v>
       </c>
@@ -21453,7 +21453,7 @@
       </c>
       <c r="I565" s="31"/>
     </row>
-    <row r="566" spans="1:9" ht="45">
+    <row r="566" spans="1:9" ht="30">
       <c r="A566" s="29" t="s">
         <v>580</v>
       </c>
@@ -21528,7 +21528,7 @@
       </c>
       <c r="I568" s="31"/>
     </row>
-    <row r="569" spans="1:9" ht="30">
+    <row r="569" spans="1:9">
       <c r="A569" s="29" t="s">
         <v>583</v>
       </c>
@@ -21553,7 +21553,7 @@
       </c>
       <c r="I569" s="31"/>
     </row>
-    <row r="570" spans="1:9" ht="45">
+    <row r="570" spans="1:9" ht="30">
       <c r="A570" s="29" t="s">
         <v>584</v>
       </c>
@@ -21578,7 +21578,7 @@
       </c>
       <c r="I570" s="31"/>
     </row>
-    <row r="571" spans="1:9" ht="30">
+    <row r="571" spans="1:9">
       <c r="A571" s="29" t="s">
         <v>585</v>
       </c>
@@ -21655,7 +21655,7 @@
       </c>
       <c r="I573" s="31"/>
     </row>
-    <row r="574" spans="1:9" ht="60">
+    <row r="574" spans="1:9" ht="45">
       <c r="A574" s="29" t="s">
         <v>588</v>
       </c>
@@ -21732,7 +21732,7 @@
       </c>
       <c r="I576" s="31"/>
     </row>
-    <row r="577" spans="1:9" ht="75">
+    <row r="577" spans="1:9" ht="60">
       <c r="A577" s="29" t="s">
         <v>591</v>
       </c>
@@ -21782,7 +21782,7 @@
       </c>
       <c r="I578" s="31"/>
     </row>
-    <row r="579" spans="1:9" ht="45">
+    <row r="579" spans="1:9" ht="30">
       <c r="A579" s="29" t="s">
         <v>593</v>
       </c>
@@ -21859,7 +21859,7 @@
       </c>
       <c r="I581" s="31"/>
     </row>
-    <row r="582" spans="1:9" ht="30">
+    <row r="582" spans="1:9">
       <c r="A582" s="29" t="s">
         <v>596</v>
       </c>
@@ -21884,7 +21884,7 @@
       </c>
       <c r="I582" s="31"/>
     </row>
-    <row r="583" spans="1:9" ht="30">
+    <row r="583" spans="1:9">
       <c r="A583" s="29" t="s">
         <v>597</v>
       </c>
@@ -21938,7 +21938,7 @@
       </c>
       <c r="I584" s="31"/>
     </row>
-    <row r="585" spans="1:9" ht="30">
+    <row r="585" spans="1:9">
       <c r="A585" s="29" t="s">
         <v>599</v>
       </c>
@@ -21990,7 +21990,7 @@
       </c>
       <c r="I586" s="31"/>
     </row>
-    <row r="587" spans="1:9" ht="30">
+    <row r="587" spans="1:9">
       <c r="A587" s="29" t="s">
         <v>601</v>
       </c>
@@ -22015,7 +22015,7 @@
       </c>
       <c r="I587" s="31"/>
     </row>
-    <row r="588" spans="1:9" ht="45">
+    <row r="588" spans="1:9" ht="30">
       <c r="A588" s="29" t="s">
         <v>602</v>
       </c>
@@ -22142,7 +22142,7 @@
       </c>
       <c r="I592" s="31"/>
     </row>
-    <row r="593" spans="1:9" ht="45">
+    <row r="593" spans="1:9" ht="30">
       <c r="A593" s="29" t="s">
         <v>607</v>
       </c>
@@ -22192,7 +22192,7 @@
       </c>
       <c r="I594" s="31"/>
     </row>
-    <row r="595" spans="1:9" ht="30">
+    <row r="595" spans="1:9">
       <c r="A595" s="29" t="s">
         <v>609</v>
       </c>
@@ -22217,7 +22217,7 @@
       </c>
       <c r="I595" s="31"/>
     </row>
-    <row r="596" spans="1:9" ht="30">
+    <row r="596" spans="1:9">
       <c r="A596" s="29" t="s">
         <v>610</v>
       </c>
@@ -22321,7 +22321,7 @@
       </c>
       <c r="I599" s="31"/>
     </row>
-    <row r="600" spans="1:9" ht="30">
+    <row r="600" spans="1:9">
       <c r="A600" s="29" t="s">
         <v>614</v>
       </c>
@@ -22423,7 +22423,7 @@
         <v>1588</v>
       </c>
     </row>
-    <row r="604" spans="1:9" ht="30">
+    <row r="604" spans="1:9">
       <c r="A604" s="29" t="s">
         <v>618</v>
       </c>
@@ -22448,7 +22448,7 @@
       </c>
       <c r="I604" s="31"/>
     </row>
-    <row r="605" spans="1:9" ht="30">
+    <row r="605" spans="1:9">
       <c r="A605" s="29" t="s">
         <v>619</v>
       </c>
@@ -22529,7 +22529,7 @@
       </c>
       <c r="I607" s="31"/>
     </row>
-    <row r="608" spans="1:9" ht="30">
+    <row r="608" spans="1:9">
       <c r="A608" s="29" t="s">
         <v>622</v>
       </c>
@@ -22554,7 +22554,7 @@
       </c>
       <c r="I608" s="31"/>
     </row>
-    <row r="609" spans="1:9" ht="30">
+    <row r="609" spans="1:9">
       <c r="A609" s="29" t="s">
         <v>623</v>
       </c>
@@ -22604,7 +22604,7 @@
       </c>
       <c r="I610" s="31"/>
     </row>
-    <row r="611" spans="1:9" ht="45">
+    <row r="611" spans="1:9" ht="30">
       <c r="A611" s="29" t="s">
         <v>625</v>
       </c>
@@ -22654,7 +22654,7 @@
       </c>
       <c r="I612" s="31"/>
     </row>
-    <row r="613" spans="1:9" ht="30">
+    <row r="613" spans="1:9">
       <c r="A613" s="29" t="s">
         <v>627</v>
       </c>
@@ -22679,7 +22679,7 @@
       </c>
       <c r="I613" s="31"/>
     </row>
-    <row r="614" spans="1:9" ht="30">
+    <row r="614" spans="1:9">
       <c r="A614" s="29" t="s">
         <v>628</v>
       </c>
@@ -22706,7 +22706,7 @@
       </c>
       <c r="I614" s="31"/>
     </row>
-    <row r="615" spans="1:9" ht="30">
+    <row r="615" spans="1:9">
       <c r="A615" s="29" t="s">
         <v>629</v>
       </c>
@@ -22733,7 +22733,7 @@
       </c>
       <c r="I615" s="31"/>
     </row>
-    <row r="616" spans="1:9" ht="30">
+    <row r="616" spans="1:9">
       <c r="A616" s="29" t="s">
         <v>630</v>
       </c>
@@ -22760,7 +22760,7 @@
       </c>
       <c r="I616" s="31"/>
     </row>
-    <row r="617" spans="1:9" ht="30">
+    <row r="617" spans="1:9">
       <c r="A617" s="29" t="s">
         <v>631</v>
       </c>
@@ -22810,7 +22810,7 @@
       </c>
       <c r="I618" s="31"/>
     </row>
-    <row r="619" spans="1:9" ht="45">
+    <row r="619" spans="1:9" ht="30">
       <c r="A619" s="29" t="s">
         <v>633</v>
       </c>
@@ -22860,7 +22860,7 @@
       </c>
       <c r="I620" s="31"/>
     </row>
-    <row r="621" spans="1:9" ht="90">
+    <row r="621" spans="1:9" ht="75">
       <c r="A621" s="29" t="s">
         <v>635</v>
       </c>
@@ -22910,7 +22910,7 @@
       </c>
       <c r="I622" s="31"/>
     </row>
-    <row r="623" spans="1:9" ht="30">
+    <row r="623" spans="1:9">
       <c r="A623" s="29" t="s">
         <v>637</v>
       </c>
@@ -23016,7 +23016,7 @@
       </c>
       <c r="I626" s="31"/>
     </row>
-    <row r="627" spans="1:9" ht="30">
+    <row r="627" spans="1:9">
       <c r="A627" s="29" t="s">
         <v>641</v>
       </c>
@@ -23041,7 +23041,7 @@
       </c>
       <c r="I627" s="31"/>
     </row>
-    <row r="628" spans="1:9" ht="45">
+    <row r="628" spans="1:9" ht="30">
       <c r="A628" s="29" t="s">
         <v>642</v>
       </c>
@@ -23066,7 +23066,7 @@
       </c>
       <c r="I628" s="31"/>
     </row>
-    <row r="629" spans="1:9" ht="30">
+    <row r="629" spans="1:9">
       <c r="A629" s="29" t="s">
         <v>643</v>
       </c>
@@ -23166,7 +23166,7 @@
       </c>
       <c r="I632" s="31"/>
     </row>
-    <row r="633" spans="1:9" ht="60">
+    <row r="633" spans="1:9" ht="45">
       <c r="A633" s="29" t="s">
         <v>647</v>
       </c>
@@ -23268,7 +23268,7 @@
         <v>15</v>
       </c>
       <c r="H636" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I636" s="31"/>
     </row>
@@ -23401,7 +23401,7 @@
       </c>
       <c r="I641" s="31"/>
     </row>
-    <row r="642" spans="1:9" ht="45">
+    <row r="642" spans="1:9" ht="30">
       <c r="A642" s="29" t="s">
         <v>656</v>
       </c>
@@ -23451,7 +23451,7 @@
       </c>
       <c r="I643" s="31"/>
     </row>
-    <row r="644" spans="1:9" ht="45">
+    <row r="644" spans="1:9" ht="30">
       <c r="A644" s="29" t="s">
         <v>658</v>
       </c>
@@ -23476,7 +23476,7 @@
       </c>
       <c r="I644" s="31"/>
     </row>
-    <row r="645" spans="1:9" ht="45">
+    <row r="645" spans="1:9" ht="30">
       <c r="A645" s="29" t="s">
         <v>659</v>
       </c>
@@ -23501,7 +23501,7 @@
       </c>
       <c r="I645" s="31"/>
     </row>
-    <row r="646" spans="1:9" ht="60">
+    <row r="646" spans="1:9" ht="45">
       <c r="A646" s="29" t="s">
         <v>660</v>
       </c>
@@ -23601,7 +23601,7 @@
       </c>
       <c r="I649" s="31"/>
     </row>
-    <row r="650" spans="1:9" ht="30">
+    <row r="650" spans="1:9">
       <c r="A650" s="29" t="s">
         <v>664</v>
       </c>
@@ -23626,7 +23626,7 @@
       </c>
       <c r="I650" s="31"/>
     </row>
-    <row r="651" spans="1:9" ht="45">
+    <row r="651" spans="1:9" ht="30">
       <c r="A651" s="22" t="s">
         <v>665</v>
       </c>
@@ -23703,7 +23703,7 @@
       </c>
       <c r="I653" s="31"/>
     </row>
-    <row r="654" spans="1:9" ht="30">
+    <row r="654" spans="1:9">
       <c r="A654" s="29" t="s">
         <v>668</v>
       </c>
@@ -23757,7 +23757,7 @@
       </c>
       <c r="I655" s="31"/>
     </row>
-    <row r="656" spans="1:9" ht="30">
+    <row r="656" spans="1:9">
       <c r="A656" s="29" t="s">
         <v>670</v>
       </c>
@@ -23807,7 +23807,7 @@
       </c>
       <c r="I657" s="31"/>
     </row>
-    <row r="658" spans="1:9" ht="45">
+    <row r="658" spans="1:9" ht="30">
       <c r="A658" s="29" t="s">
         <v>672</v>
       </c>
@@ -23882,7 +23882,7 @@
       </c>
       <c r="I660" s="31"/>
     </row>
-    <row r="661" spans="1:9" ht="60">
+    <row r="661" spans="1:9" ht="45">
       <c r="A661" s="29" t="s">
         <v>675</v>
       </c>
@@ -24057,7 +24057,7 @@
       </c>
       <c r="I667" s="31"/>
     </row>
-    <row r="668" spans="1:9" ht="30">
+    <row r="668" spans="1:9">
       <c r="A668" s="29" t="s">
         <v>682</v>
       </c>
@@ -24084,7 +24084,7 @@
       </c>
       <c r="I668" s="31"/>
     </row>
-    <row r="669" spans="1:9" ht="30">
+    <row r="669" spans="1:9">
       <c r="A669" s="29" t="s">
         <v>683</v>
       </c>
@@ -24111,7 +24111,7 @@
       </c>
       <c r="I669" s="31"/>
     </row>
-    <row r="670" spans="1:9" ht="30">
+    <row r="670" spans="1:9">
       <c r="A670" s="29" t="s">
         <v>684</v>
       </c>
@@ -24136,7 +24136,7 @@
       </c>
       <c r="I670" s="31"/>
     </row>
-    <row r="671" spans="1:9" ht="45">
+    <row r="671" spans="1:9" ht="30">
       <c r="A671" s="29" t="s">
         <v>685</v>
       </c>
@@ -24186,7 +24186,7 @@
       </c>
       <c r="I672" s="31"/>
     </row>
-    <row r="673" spans="1:9" ht="45">
+    <row r="673" spans="1:9" ht="30">
       <c r="A673" s="29" t="s">
         <v>687</v>
       </c>
@@ -24261,7 +24261,7 @@
       </c>
       <c r="I675" s="31"/>
     </row>
-    <row r="676" spans="1:9" ht="30">
+    <row r="676" spans="1:9">
       <c r="A676" s="29" t="s">
         <v>690</v>
       </c>
@@ -24288,7 +24288,7 @@
       </c>
       <c r="I676" s="31"/>
     </row>
-    <row r="677" spans="1:9" ht="30">
+    <row r="677" spans="1:9">
       <c r="A677" s="29" t="s">
         <v>691</v>
       </c>
@@ -24315,7 +24315,7 @@
       </c>
       <c r="I677" s="31"/>
     </row>
-    <row r="678" spans="1:9" ht="30">
+    <row r="678" spans="1:9">
       <c r="A678" s="29" t="s">
         <v>692</v>
       </c>
@@ -24342,7 +24342,7 @@
       </c>
       <c r="I678" s="31"/>
     </row>
-    <row r="679" spans="1:9" ht="30">
+    <row r="679" spans="1:9">
       <c r="A679" s="29" t="s">
         <v>693</v>
       </c>
@@ -24392,7 +24392,7 @@
       </c>
       <c r="I680" s="31"/>
     </row>
-    <row r="681" spans="1:9" ht="45">
+    <row r="681" spans="1:9" ht="30">
       <c r="A681" s="29" t="s">
         <v>695</v>
       </c>
@@ -24417,7 +24417,7 @@
       </c>
       <c r="I681" s="31"/>
     </row>
-    <row r="682" spans="1:9" ht="60">
+    <row r="682" spans="1:9" ht="45">
       <c r="A682" s="29" t="s">
         <v>696</v>
       </c>
@@ -24519,7 +24519,7 @@
         <v>1590</v>
       </c>
     </row>
-    <row r="686" spans="1:9" ht="60">
+    <row r="686" spans="1:9" ht="45">
       <c r="A686" s="29" t="s">
         <v>700</v>
       </c>
@@ -24573,7 +24573,7 @@
         <v>1591</v>
       </c>
     </row>
-    <row r="688" spans="1:9" ht="75">
+    <row r="688" spans="1:9" ht="60">
       <c r="A688" s="29" t="s">
         <v>702</v>
       </c>
@@ -24594,7 +24594,7 @@
         <v>15</v>
       </c>
       <c r="H688" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I688" s="31"/>
     </row>
@@ -24779,7 +24779,7 @@
       </c>
       <c r="I695" s="31"/>
     </row>
-    <row r="696" spans="1:9" ht="30">
+    <row r="696" spans="1:9">
       <c r="A696" s="29" t="s">
         <v>710</v>
       </c>
@@ -24804,7 +24804,7 @@
       </c>
       <c r="I696" s="31"/>
     </row>
-    <row r="697" spans="1:9" ht="30">
+    <row r="697" spans="1:9">
       <c r="A697" s="29" t="s">
         <v>711</v>
       </c>
@@ -24904,7 +24904,7 @@
       </c>
       <c r="I700" s="31"/>
     </row>
-    <row r="701" spans="1:9" ht="30">
+    <row r="701" spans="1:9">
       <c r="A701" s="29" t="s">
         <v>715</v>
       </c>
@@ -24929,7 +24929,7 @@
       </c>
       <c r="I701" s="31"/>
     </row>
-    <row r="702" spans="1:9" ht="45">
+    <row r="702" spans="1:9" ht="30">
       <c r="A702" s="29" t="s">
         <v>716</v>
       </c>
@@ -25006,7 +25006,7 @@
       </c>
       <c r="I704" s="31"/>
     </row>
-    <row r="705" spans="1:9" ht="45">
+    <row r="705" spans="1:9" ht="30">
       <c r="A705" s="29" t="s">
         <v>719</v>
       </c>
@@ -25081,7 +25081,7 @@
       </c>
       <c r="I707" s="35"/>
     </row>
-    <row r="708" spans="1:9" ht="45">
+    <row r="708" spans="1:9" ht="30">
       <c r="A708" s="29" t="s">
         <v>721</v>
       </c>
@@ -25131,7 +25131,7 @@
       </c>
       <c r="I709" s="31"/>
     </row>
-    <row r="710" spans="1:9" ht="45">
+    <row r="710" spans="1:9" ht="30">
       <c r="A710" s="29" t="s">
         <v>723</v>
       </c>
@@ -25181,7 +25181,7 @@
       </c>
       <c r="I711" s="31"/>
     </row>
-    <row r="712" spans="1:9" ht="45">
+    <row r="712" spans="1:9" ht="30">
       <c r="A712" s="29" t="s">
         <v>725</v>
       </c>
@@ -25256,7 +25256,7 @@
       </c>
       <c r="I714" s="31"/>
     </row>
-    <row r="715" spans="1:9" ht="60">
+    <row r="715" spans="1:9" ht="45">
       <c r="A715" s="29" t="s">
         <v>728</v>
       </c>
@@ -25281,7 +25281,7 @@
       </c>
       <c r="I715" s="31"/>
     </row>
-    <row r="716" spans="1:9" ht="30">
+    <row r="716" spans="1:9">
       <c r="A716" s="29" t="s">
         <v>729</v>
       </c>
@@ -25356,7 +25356,7 @@
       </c>
       <c r="I718" s="31"/>
     </row>
-    <row r="719" spans="1:9" ht="30">
+    <row r="719" spans="1:9">
       <c r="A719" s="29" t="s">
         <v>732</v>
       </c>
@@ -25381,7 +25381,7 @@
       </c>
       <c r="I719" s="31"/>
     </row>
-    <row r="720" spans="1:9" ht="30">
+    <row r="720" spans="1:9">
       <c r="A720" s="29" t="s">
         <v>733</v>
       </c>
@@ -25406,7 +25406,7 @@
       </c>
       <c r="I720" s="31"/>
     </row>
-    <row r="721" spans="1:9" ht="30">
+    <row r="721" spans="1:9">
       <c r="A721" s="29" t="s">
         <v>734</v>
       </c>
@@ -25481,7 +25481,7 @@
       </c>
       <c r="I723" s="31"/>
     </row>
-    <row r="724" spans="1:9" ht="30">
+    <row r="724" spans="1:9">
       <c r="A724" s="29" t="s">
         <v>737</v>
       </c>
@@ -25531,7 +25531,7 @@
       </c>
       <c r="I725" s="31"/>
     </row>
-    <row r="726" spans="1:9" ht="30">
+    <row r="726" spans="1:9">
       <c r="A726" s="29" t="s">
         <v>739</v>
       </c>
@@ -25581,7 +25581,7 @@
       </c>
       <c r="I727" s="31"/>
     </row>
-    <row r="728" spans="1:9" ht="45">
+    <row r="728" spans="1:9" ht="30">
       <c r="A728" s="29" t="s">
         <v>741</v>
       </c>
@@ -25656,7 +25656,7 @@
       </c>
       <c r="I730" s="31"/>
     </row>
-    <row r="731" spans="1:9" ht="30">
+    <row r="731" spans="1:9">
       <c r="A731" s="29" t="s">
         <v>744</v>
       </c>
@@ -25706,7 +25706,7 @@
       </c>
       <c r="I732" s="31"/>
     </row>
-    <row r="733" spans="1:9" ht="30">
+    <row r="733" spans="1:9">
       <c r="A733" s="29" t="s">
         <v>746</v>
       </c>
@@ -25756,7 +25756,7 @@
       </c>
       <c r="I734" s="31"/>
     </row>
-    <row r="735" spans="1:9" ht="45">
+    <row r="735" spans="1:9" ht="30">
       <c r="A735" s="29" t="s">
         <v>748</v>
       </c>
@@ -25806,7 +25806,7 @@
       </c>
       <c r="I736" s="31"/>
     </row>
-    <row r="737" spans="1:9" ht="45">
+    <row r="737" spans="1:9" ht="30">
       <c r="A737" s="29" t="s">
         <v>750</v>
       </c>
@@ -25831,7 +25831,7 @@
       </c>
       <c r="I737" s="31"/>
     </row>
-    <row r="738" spans="1:9" ht="30">
+    <row r="738" spans="1:9">
       <c r="A738" s="29" t="s">
         <v>751</v>
       </c>
@@ -25881,7 +25881,7 @@
       </c>
       <c r="I739" s="31"/>
     </row>
-    <row r="740" spans="1:9" ht="30">
+    <row r="740" spans="1:9">
       <c r="A740" s="29" t="s">
         <v>753</v>
       </c>
@@ -25906,7 +25906,7 @@
       </c>
       <c r="I740" s="31"/>
     </row>
-    <row r="741" spans="1:9" ht="30">
+    <row r="741" spans="1:9">
       <c r="A741" s="29" t="s">
         <v>754</v>
       </c>
@@ -25956,7 +25956,7 @@
       </c>
       <c r="I742" s="31"/>
     </row>
-    <row r="743" spans="1:9" ht="45">
+    <row r="743" spans="1:9" ht="30">
       <c r="A743" s="29" t="s">
         <v>756</v>
       </c>
@@ -25981,7 +25981,7 @@
       </c>
       <c r="I743" s="31"/>
     </row>
-    <row r="744" spans="1:9" ht="45">
+    <row r="744" spans="1:9" ht="30">
       <c r="A744" s="29" t="s">
         <v>757</v>
       </c>
@@ -26006,7 +26006,7 @@
       </c>
       <c r="I744" s="31"/>
     </row>
-    <row r="745" spans="1:9" ht="30">
+    <row r="745" spans="1:9">
       <c r="A745" s="29" t="s">
         <v>758</v>
       </c>
@@ -26056,7 +26056,7 @@
       </c>
       <c r="I746" s="31"/>
     </row>
-    <row r="747" spans="1:9" ht="30">
+    <row r="747" spans="1:9">
       <c r="A747" s="29" t="s">
         <v>760</v>
       </c>
@@ -26081,7 +26081,7 @@
       </c>
       <c r="I747" s="31"/>
     </row>
-    <row r="748" spans="1:9" ht="30">
+    <row r="748" spans="1:9">
       <c r="A748" s="29" t="s">
         <v>761</v>
       </c>
@@ -26131,7 +26131,7 @@
       </c>
       <c r="I749" s="31"/>
     </row>
-    <row r="750" spans="1:9" ht="45">
+    <row r="750" spans="1:9" ht="30">
       <c r="A750" s="29" t="s">
         <v>763</v>
       </c>
@@ -26376,7 +26376,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="759" spans="1:9" ht="60">
+    <row r="759" spans="1:9" ht="45">
       <c r="A759" s="29" t="s">
         <v>796</v>
       </c>
@@ -26432,7 +26432,7 @@
         <v>1621</v>
       </c>
     </row>
-    <row r="761" spans="1:9" ht="75">
+    <row r="761" spans="1:9" ht="60">
       <c r="A761" s="29" t="s">
         <v>767</v>
       </c>
@@ -26515,7 +26515,7 @@
         <v>1648</v>
       </c>
     </row>
-    <row r="764" spans="1:9" ht="75">
+    <row r="764" spans="1:9" ht="60">
       <c r="A764" s="29" t="s">
         <v>770</v>
       </c>
@@ -26598,7 +26598,7 @@
         <v>1649</v>
       </c>
     </row>
-    <row r="767" spans="1:9" ht="75">
+    <row r="767" spans="1:9" ht="60">
       <c r="A767" s="29" t="s">
         <v>773</v>
       </c>
@@ -26841,7 +26841,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="776" spans="1:9" ht="45">
+    <row r="776" spans="1:9" ht="30">
       <c r="A776" s="29" t="s">
         <v>777</v>
       </c>
@@ -26893,7 +26893,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="778" spans="1:9" ht="60">
+    <row r="778" spans="1:9" ht="45">
       <c r="A778" s="22" t="s">
         <v>779</v>
       </c>
@@ -26945,7 +26945,7 @@
         <v>15</v>
       </c>
       <c r="H779" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I779" s="31" t="s">
         <v>1593</v>
@@ -27003,7 +27003,7 @@
       </c>
       <c r="I781" s="31"/>
     </row>
-    <row r="782" spans="1:9" ht="60">
+    <row r="782" spans="1:9" ht="45">
       <c r="A782" s="29" t="s">
         <v>782</v>
       </c>
@@ -27030,7 +27030,7 @@
         <v>1625</v>
       </c>
     </row>
-    <row r="783" spans="1:9" ht="45">
+    <row r="783" spans="1:9" ht="30">
       <c r="A783" s="29" t="s">
         <v>783</v>
       </c>
@@ -27109,7 +27109,7 @@
         <v>1625</v>
       </c>
     </row>
-    <row r="786" spans="1:9" ht="90">
+    <row r="786" spans="1:9" ht="75">
       <c r="A786" s="29" t="s">
         <v>802</v>
       </c>
@@ -27138,7 +27138,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="787" spans="1:9" ht="75">
+    <row r="787" spans="1:9" ht="60">
       <c r="A787" s="29" t="s">
         <v>801</v>
       </c>
@@ -27167,7 +27167,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="788" spans="1:9" ht="75">
+    <row r="788" spans="1:9" ht="60">
       <c r="A788" s="29" t="s">
         <v>803</v>
       </c>
@@ -27196,7 +27196,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="789" spans="1:9" ht="90">
+    <row r="789" spans="1:9" ht="75">
       <c r="A789" s="29" t="s">
         <v>804</v>
       </c>
@@ -27225,7 +27225,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="790" spans="1:9" ht="75">
+    <row r="790" spans="1:9" ht="60">
       <c r="A790" s="29" t="s">
         <v>805</v>
       </c>
@@ -27254,7 +27254,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="791" spans="1:9" ht="90">
+    <row r="791" spans="1:9" ht="75">
       <c r="A791" s="29" t="s">
         <v>806</v>
       </c>
@@ -27283,7 +27283,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="792" spans="1:9" ht="60">
+    <row r="792" spans="1:9" ht="45">
       <c r="A792" s="22" t="s">
         <v>1673</v>
       </c>
@@ -27681,7 +27681,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="806" spans="1:9" ht="75">
+    <row r="806" spans="1:9" ht="60">
       <c r="A806" s="29" t="s">
         <v>817</v>
       </c>
@@ -27768,7 +27768,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="809" spans="1:9" ht="60">
+    <row r="809" spans="1:9" ht="45">
       <c r="A809" s="29" t="s">
         <v>822</v>
       </c>
@@ -27824,7 +27824,7 @@
       </c>
       <c r="I810" s="31"/>
     </row>
-    <row r="811" spans="1:9" ht="60">
+    <row r="811" spans="1:9" ht="45">
       <c r="A811" s="29" t="s">
         <v>824</v>
       </c>
@@ -27876,7 +27876,7 @@
       </c>
       <c r="I812" s="31"/>
     </row>
-    <row r="813" spans="1:9" ht="60">
+    <row r="813" spans="1:9" ht="45">
       <c r="A813" s="29" t="s">
         <v>826</v>
       </c>
@@ -27905,7 +27905,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="814" spans="1:9" ht="60">
+    <row r="814" spans="1:9" ht="45">
       <c r="A814" s="29" t="s">
         <v>827</v>
       </c>
@@ -27934,7 +27934,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="815" spans="1:9" ht="60">
+    <row r="815" spans="1:9" ht="45">
       <c r="A815" s="29" t="s">
         <v>828</v>
       </c>
@@ -27963,7 +27963,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="816" spans="1:9" ht="60">
+    <row r="816" spans="1:9" ht="45">
       <c r="A816" s="22" t="s">
         <v>1682</v>
       </c>
@@ -27990,7 +27990,7 @@
       </c>
       <c r="I816" s="31"/>
     </row>
-    <row r="817" spans="1:9" ht="60">
+    <row r="817" spans="1:9" ht="45">
       <c r="A817" s="29" t="s">
         <v>829</v>
       </c>
@@ -28017,7 +28017,7 @@
       </c>
       <c r="I817" s="31"/>
     </row>
-    <row r="818" spans="1:9" ht="60">
+    <row r="818" spans="1:9" ht="45">
       <c r="A818" s="29" t="s">
         <v>830</v>
       </c>
@@ -28046,7 +28046,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="819" spans="1:9" ht="45">
+    <row r="819" spans="1:9" ht="30">
       <c r="A819" s="29" t="s">
         <v>787</v>
       </c>
@@ -28123,7 +28123,7 @@
       </c>
       <c r="I821" s="31"/>
     </row>
-    <row r="822" spans="1:9" ht="75">
+    <row r="822" spans="1:9" ht="60">
       <c r="A822" s="22" t="s">
         <v>1667</v>
       </c>
@@ -28148,7 +28148,7 @@
       </c>
       <c r="I822" s="31"/>
     </row>
-    <row r="823" spans="1:9" ht="75">
+    <row r="823" spans="1:9" ht="60">
       <c r="A823" s="22" t="s">
         <v>1957</v>
       </c>
@@ -28173,7 +28173,7 @@
       </c>
       <c r="I823" s="31"/>
     </row>
-    <row r="824" spans="1:9" ht="45">
+    <row r="824" spans="1:9" ht="30">
       <c r="A824" s="22" t="s">
         <v>1669</v>
       </c>
@@ -28227,7 +28227,7 @@
       </c>
       <c r="I825" s="31"/>
     </row>
-    <row r="826" spans="1:9" ht="75">
+    <row r="826" spans="1:9" ht="60">
       <c r="A826" s="29" t="s">
         <v>831</v>
       </c>
@@ -28256,7 +28256,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="827" spans="1:9" ht="75">
+    <row r="827" spans="1:9" ht="60">
       <c r="A827" s="22" t="s">
         <v>1680</v>
       </c>
@@ -28285,7 +28285,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="828" spans="1:9" ht="75">
+    <row r="828" spans="1:9" ht="60">
       <c r="A828" s="22" t="s">
         <v>1681</v>
       </c>
@@ -28314,7 +28314,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="829" spans="1:9" ht="75">
+    <row r="829" spans="1:9" ht="60">
       <c r="A829" s="22" t="s">
         <v>1679</v>
       </c>
@@ -28341,7 +28341,7 @@
       </c>
       <c r="I829" s="31"/>
     </row>
-    <row r="830" spans="1:9" ht="75">
+    <row r="830" spans="1:9" ht="60">
       <c r="A830" s="29" t="s">
         <v>832</v>
       </c>
@@ -28370,7 +28370,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="831" spans="1:9" ht="75">
+    <row r="831" spans="1:9" ht="60">
       <c r="A831" s="29" t="s">
         <v>833</v>
       </c>
@@ -28505,7 +28505,7 @@
       </c>
       <c r="I835" s="31"/>
     </row>
-    <row r="836" spans="1:9" ht="75">
+    <row r="836" spans="1:9" ht="60">
       <c r="A836" s="29" t="s">
         <v>807</v>
       </c>
@@ -28679,7 +28679,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="842" spans="1:9" ht="60">
+    <row r="842" spans="1:9" ht="45">
       <c r="A842" s="29" t="s">
         <v>825</v>
       </c>
@@ -28810,7 +28810,7 @@
       </c>
       <c r="I846" s="31"/>
     </row>
-    <row r="847" spans="1:9" ht="75">
+    <row r="847" spans="1:9" ht="60">
       <c r="A847" s="29" t="s">
         <v>838</v>
       </c>
@@ -28885,7 +28885,7 @@
       </c>
       <c r="I849" s="31"/>
     </row>
-    <row r="850" spans="1:9" ht="45">
+    <row r="850" spans="1:9" ht="30">
       <c r="A850" s="29" t="s">
         <v>841</v>
       </c>
@@ -28910,7 +28910,7 @@
       </c>
       <c r="I850" s="31"/>
     </row>
-    <row r="851" spans="1:9" ht="75">
+    <row r="851" spans="1:9" ht="60">
       <c r="A851" s="29" t="s">
         <v>842</v>
       </c>
@@ -28960,7 +28960,7 @@
       </c>
       <c r="I852" s="31"/>
     </row>
-    <row r="853" spans="1:9" ht="30">
+    <row r="853" spans="1:9">
       <c r="A853" s="29" t="s">
         <v>844</v>
       </c>
@@ -29045,6 +29045,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -29052,11 +29057,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:I855">

</xml_diff>

<commit_message>
[MS-OXCTABL] Update model to capture requirement R908
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCTABL/MS-OXCTABL_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCTABL/MS-OXCTABL_RequirementSpecification.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6126" uniqueCount="1958">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6127" uniqueCount="1958">
   <si>
     <t>Req ID</t>
   </si>
@@ -6427,6 +6427,21 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -6450,21 +6465,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7407,127 +7407,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -7540,12 +7540,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -7558,12 +7558,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -7576,12 +7576,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -7594,60 +7594,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -28011,9 +28011,11 @@
         <v>15</v>
       </c>
       <c r="H817" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="I817" s="31"/>
+        <v>20</v>
+      </c>
+      <c r="I817" s="31" t="s">
+        <v>1593</v>
+      </c>
     </row>
     <row r="818" spans="1:9" ht="45">
       <c r="A818" s="29" t="s">
@@ -29043,11 +29045,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -29055,6 +29052,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:I855">

</xml_diff>

<commit_message>
update according to the comments
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCTABL/MS-OXCTABL_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCTABL/MS-OXCTABL_RequirementSpecification.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6130" uniqueCount="1959">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6134" uniqueCount="1959">
   <si>
     <t>Req ID</t>
   </si>
@@ -6439,6 +6439,21 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -6463,158 +6478,11 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="43">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -6953,6 +6821,138 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -7082,34 +7082,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I856" tableType="xml" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41" headerRowCellStyle="Normal" dataCellStyle="Normal" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I856" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" headerRowCellStyle="Normal" dataCellStyle="Normal" connectionId="1">
   <autoFilter ref="A19:I856"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="40" dataCellStyle="Normal">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="39" dataCellStyle="Normal">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="38" dataCellStyle="Normal">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="37" dataCellStyle="Normal">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="36" dataCellStyle="Normal">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="35" dataCellStyle="Normal">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="34" dataCellStyle="Normal">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="33" dataCellStyle="Normal">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="32">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -7118,12 +7118,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="26"/>
-    <tableColumn id="2" name="Test" dataDxfId="25"/>
-    <tableColumn id="3" name="Description" dataDxfId="24"/>
+    <tableColumn id="1" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7507,127 +7507,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -7640,12 +7640,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -7658,12 +7658,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -7676,12 +7676,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -7694,60 +7694,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -28052,9 +28052,11 @@
         <v>15</v>
       </c>
       <c r="H815" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="I815" s="31"/>
+        <v>20</v>
+      </c>
+      <c r="I815" s="31" t="s">
+        <v>1589</v>
+      </c>
     </row>
     <row r="816" spans="1:9" ht="45">
       <c r="A816" s="29" t="s">
@@ -28164,9 +28166,11 @@
         <v>15</v>
       </c>
       <c r="H819" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="I819" s="31"/>
+        <v>20</v>
+      </c>
+      <c r="I819" s="31" t="s">
+        <v>1589</v>
+      </c>
     </row>
     <row r="820" spans="1:9" ht="30">
       <c r="A820" s="29" t="s">
@@ -28401,9 +28405,11 @@
         <v>15</v>
       </c>
       <c r="H828" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="I828" s="31"/>
+        <v>20</v>
+      </c>
+      <c r="I828" s="31" t="s">
+        <v>1589</v>
+      </c>
     </row>
     <row r="829" spans="1:9" ht="60">
       <c r="A829" s="22" t="s">
@@ -28513,9 +28519,11 @@
         <v>15</v>
       </c>
       <c r="H832" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="I832" s="31"/>
+        <v>20</v>
+      </c>
+      <c r="I832" s="31" t="s">
+        <v>1589</v>
+      </c>
     </row>
     <row r="833" spans="1:9" ht="60">
       <c r="A833" s="22" t="s">
@@ -29163,11 +29171,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -29175,95 +29178,100 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:I333 A335:I856">
-    <cfRule type="expression" dxfId="23" priority="135">
+    <cfRule type="expression" dxfId="42" priority="135">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="136">
+    <cfRule type="expression" dxfId="41" priority="136">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="143">
+    <cfRule type="expression" dxfId="40" priority="143">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:I333 A335:I856">
-    <cfRule type="expression" dxfId="20" priority="89">
+    <cfRule type="expression" dxfId="39" priority="89">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="90">
+    <cfRule type="expression" dxfId="38" priority="90">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="91">
+    <cfRule type="expression" dxfId="37" priority="91">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F333 F335:F856">
-    <cfRule type="expression" dxfId="17" priority="95">
+    <cfRule type="expression" dxfId="36" priority="95">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="96">
+    <cfRule type="expression" dxfId="35" priority="96">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A334:D334 F334:J334">
-    <cfRule type="expression" dxfId="15" priority="14">
+    <cfRule type="expression" dxfId="34" priority="14">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="15">
+    <cfRule type="expression" dxfId="33" priority="15">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="16">
+    <cfRule type="expression" dxfId="32" priority="16">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A334:D334 F334:J334">
-    <cfRule type="expression" dxfId="12" priority="9">
+    <cfRule type="expression" dxfId="31" priority="9">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="10">
+    <cfRule type="expression" dxfId="30" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="29" priority="11">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G334">
-    <cfRule type="expression" dxfId="9" priority="12">
+    <cfRule type="expression" dxfId="28" priority="12">
       <formula>NOT(VLOOKUP(G334,$A$13:$C$16,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="13">
+    <cfRule type="expression" dxfId="27" priority="13">
       <formula>(VLOOKUP(G334,$A$13:$C$16,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E334">
-    <cfRule type="expression" dxfId="7" priority="6">
+    <cfRule type="expression" dxfId="26" priority="6">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="25" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="8">
+    <cfRule type="expression" dxfId="24" priority="8">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E334">
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="23" priority="3">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="22" priority="4">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="5">
+    <cfRule type="expression" dxfId="21" priority="5">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F334">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="20" priority="1">
       <formula>NOT(VLOOKUP(F334,$A$13:$C$16,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>(VLOOKUP(F334,$A$13:$C$16,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29281,7 +29289,7 @@
       <formula1>"In, Out"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H856 I334">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I334 H20:H856">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F334">

</xml_diff>